<commit_message>
Hotfix: Mon Oct 21 17:53:26 RTZ 2024
</commit_message>
<xml_diff>
--- a/files/database_tables.xlsx
+++ b/files/database_tables.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -621,26 +621,6 @@
       <c r="D12" t="inlineStr">
         <is>
           <t>Вывод всех записей таблицы</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>1164</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>hgfhgfhgfhhgfhgfhgfh</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>hgfhgfhgfhhgfhgfhgfh</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>hgfhgfhgfhhgfhgfhgfhhgfhgfhgfh</t>
         </is>
       </c>
     </row>
@@ -655,7 +635,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1481,26 +1461,6 @@
         </is>
       </c>
     </row>
-    <row r="38">
-      <c r="A38" t="n">
-        <v>2101</v>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>hgfhgfhgfhhgfhgfhgfhhgfhgfhgfh</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>hgfhgfhgfhhgfhgfhgfh</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>hgfhgfhgfhhgfhgfhgfh</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1512,7 +1472,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1522,271 +1482,251 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>add_links_commandadd_links_commandadd_links_command</t>
+          <t>Яндекс</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>add_links_commandadd_links_commandadd_links_command</t>
+          <t>https://yandex.ru/</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>add_links_commandadd_links_commandadd_links_command</t>
+          <t>Поисковая система</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Яндекс</t>
+          <t>Blueprint</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://yandex.ru/</t>
+          <t>https://dnmtechs.com/splitting-a-python-flask-app-into-multiple-files/</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Поисковая система</t>
+          <t>Разбивка приложения на части</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Blueprint</t>
+          <t>Документация CLI PowerSHell</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://dnmtechs.com/splitting-a-python-flask-app-into-multiple-files/</t>
+          <t>https://learn.microsoft.com/ru-ru/powershell/</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Разбивка приложения на части</t>
+          <t>Документация CLI PowerSHell</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Документация CLI PowerSHell</t>
+          <t>Описание библиотеки, которая позволяет работает с базой mysql</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://learn.microsoft.com/ru-ru/powershell/</t>
+          <t>https://pypi.org/project/PyMySQL/</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Документация CLI PowerSHell</t>
+          <t>Описание библиотеки, которая позволяет работает с базой mysql.</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Описание библиотеки, которая позволяет работает с базой mysql</t>
+          <t>Документация по Bootstrap</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://pypi.org/project/PyMySQL/</t>
+          <t>https://getbootstrap.com/</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Описание библиотеки, которая позволяет работает с базой mysql.</t>
+          <t>Документация по Bootstrap.</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Документация по Bootstrap</t>
+          <t>Сайт с документацией по веб-технологиям</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://getbootstrap.com/</t>
+          <t>https://developer.mozilla.org/ru/docs/Web</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Документация по Bootstrap.</t>
+          <t>Сайт с документацией по веб-технологиям.</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Сайт с документацией по веб-технологиям</t>
+          <t>Работа с gitignore</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://developer.mozilla.org/ru/docs/Web</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Сайт с документацией по веб-технологиям.</t>
-        </is>
-      </c>
+          <t>https://wiki.merionet.ru/articles/fajl-gitignore-kak-ignorirovat-fajly-i-papki-v-git</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Работа с gitignore</t>
+          <t>Красивый python</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://wiki.merionet.ru/articles/fajl-gitignore-kak-ignorirovat-fajly-i-papki-v-git</t>
+          <t>https://sky.pro/media/pep8/</t>
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Красивый python</t>
+          <t>Горячие клавиши Bash</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://sky.pro/media/pep8/</t>
+          <t>https://selectel.ru/blog/tutorials/linux-terminal-hotkeys/</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Горячие клавиши Bash</t>
+          <t>Интересный материал про bash</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://selectel.ru/blog/tutorials/linux-terminal-hotkeys/</t>
+          <t>https://linuxsimply.com/bash-scripting-tutorial/basics/</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Интересный материал про bash</t>
+          <t>Список команд Windows CMD с описанием и примерами</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://linuxsimply.com/bash-scripting-tutorial/basics/</t>
+          <t>https://ab57.ru/cmdlist.html</t>
         </is>
       </c>
       <c r="D11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Список команд Windows CMD с описанием и примерами</t>
+          <t>Работа с 7zip из командной строки</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://ab57.ru/cmdlist.html</t>
+          <t xml:space="preserve">https://www.dmosk.ru/miniinstruktions.php?mini=7zip-cmd </t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Работа с 7zip из командной строки</t>
+          <t>Как создать и запустить bat-файлы</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://www.dmosk.ru/miniinstruktions.php?mini=7zip-cmd </t>
+          <t>https://www.nic.ru/help/kak-sozdat6-i-zapustit6-bat-fajly_11640.html</t>
         </is>
       </c>
       <c r="D13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Как создать и запустить bat-файлы</t>
+          <t>Как сделать скрипт на bash</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://www.nic.ru/help/kak-sozdat6-i-zapustit6-bat-fajly_11640.html</t>
+          <t>https://selectel.ru/blog/tutorials/linux-bash-scripting-guide/</t>
         </is>
       </c>
       <c r="D14" t="inlineStr"/>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>1</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Как сделать скрипт на bash</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>https://selectel.ru/blog/tutorials/linux-bash-scripting-guide/</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1799,7 +1739,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C72"/>
+  <dimension ref="A1:C74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2880,31 +2820,61 @@
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>TestTestTestTestTestTestTestTest</t>
+          <t>mount</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>TestTestTestTestTestTestTestTest</t>
+          <t>Вывод всех подключенных дисков</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>hgfhgfhgfhhgfhgfhgfh</t>
+          <t>tar -cf flask-project.tar * &amp;&amp; mv flask-project.tar /o</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>hgfhgfhgfhhgfhgfhgfh</t>
+          <t>Скрипт архивации файлов и перенос архива на другой диск</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>114</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>tar -cf flask-project.tar *</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Создание архива всех файлов в папке</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>115</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>mv flask-project.tar /o</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Перенос файла в другой диск</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Hotfix: Tue Oct 22 17:57:11 RTZ 2024
</commit_message>
<xml_diff>
--- a/files/database_tables.xlsx
+++ b/files/database_tables.xlsx
@@ -1201,21 +1201,19 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>import sqlite3
-def create_tables():
+          <t>def create_tables():
     sql_statements = [
-        """CREATE TABLE IF NOT EXISTS main.table_name (
-                id INTEGER PRIMARY KEY autoincrement, 
-                table_name TEXT not null,
-                table_content TEXT not null
+        """CREATE TABLE IF NOT EXISTS test (
+                test_id INTEGER PRIMARY KEY autoincrement, 
+                test_name TEXT not null
         );"""]
     try:
-        with sqlite3.connect('/database1.db') as conn:
+        with conn:
             cursor = conn.cursor()
             for statement in sql_statements:
                 cursor.execute(statement)
             conn.commit()
-    except sqlite3.Error as e:
+    except connect.Error as e:
         print(e)
 if __name__ == '__main__':
     create_tables()</t>

</xml_diff>

<commit_message>
Hotfix: Thu Oct 24 17:52:23 RTZ 2024
</commit_message>
<xml_diff>
--- a/files/database_tables.xlsx
+++ b/files/database_tables.xlsx
@@ -635,7 +635,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1130,332 +1130,12 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Загрузка CSV-данных</t>
+          <t>Загрузка CSV-данных в датафрейм</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
           <t>Метод загружает csv файл с данными.</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="n">
-        <v>2090</v>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>Тестовое сообщение</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>Тестовое сообщение</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>Тестовое сообщение1</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="n">
-        <v>2092</v>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>Скрипт преобразования данных таблицы в датафрейм</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>Скрипт преобразования данных таблицы в датафрейм</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>import sqlite3
-import pandas as pd
-con = sqlite3.connect("/database1.db")
-cur = con.cursor()
-res = cur.execute("SELECT * FROM links")
-result = res.fetchall()
-df = pd.DataFrame(result, columns=[c[0] for c in cur.description])</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="n">
-        <v>2093</v>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>Скрипт добавления таблицы в базу данных</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>Скрипт добавления таблицы в базу данных</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>def create_tables():
-    sql_statements = [
-        """CREATE TABLE IF NOT EXISTS test (
-                test_id INTEGER PRIMARY KEY autoincrement, 
-                test_name TEXT not null
-        );"""]
-    try:
-        with conn:
-            cursor = conn.cursor()
-            for statement in sql_statements:
-                cursor.execute(statement)
-            conn.commit()
-    except connect.Error as e:
-        print(e)
-if __name__ == '__main__':
-    create_tables()</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="n">
-        <v>2094</v>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Скрипт удаления из таблицы баз данных определенных id </t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Скрипт удаления из таблицы баз данных определенных id </t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t># Подключаем библиотеку sqlite3
-import sqlite3
-# Подключаемся в базе данных
-con = sqlite3.connect("../database1.db")
-cur = con.cursor()
-res = cur.execute("DELETE FROM links WHERE id IN (12,13,14)")
-res.fetchall()
-con.commit()</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="n">
-        <v>2095</v>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>Скрипт очистки таблицы базы данных</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>Скрипт очистки таблицы базы данных</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>import sqlite3
-con = sqlite3.connect("/database1.db")
-cur = con.cursor()
-res = cur.execute("DROP TABLE table_name")
-con.commit()</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="n">
-        <v>2096</v>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>Скрипт удаления таблицы</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>Скрипт удаления таблицы</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>import sqlite3
-con = sqlite3.connect("/database1.db")
-cur = con.cursor()
-res = cur.execute("DROP TABLE table_name")
-con.commit()</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="n">
-        <v>2097</v>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>Скрипт вставки значений в таблицу</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>Скрипт вставки значений в таблицу</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t xml:space="preserve"># Подключаем библиотеку sqlite3
-import sqlite3
-# Подключаемся в базе данных
-con = sqlite3.connect("../database1.db")
-cur = con.cursor()
-data = (
-    {"id": None, "name": "test", "link": "test"},
-    {"id": None, "name": "test", "link": "test"},
-    {"id": None, "name": "test", "link": "test"},
-)
-cur.executemany("INSERT INTO links VALUES(:id,:name, :link)", data)
-con.commit()
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="n">
-        <v>2098</v>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>Экземпляр приложения Flask</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>Экземпляр приложения Flask с подключением внешней базы данных и пагинацией</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>import flask
-import pymysql.cursors
-from flask_paginate import Pagination, get_page_args
-app = flask.Flask(__name__)
-app.secret_key = "secret key"
-@app.errorhandler(404)
-def page_not_found(e):
-    return flask.render_template('404.html'), 404
-def get_db_connection():
-    conn = pymysql.connect(host='localhost',
-                           port=3307,
-                           user='root',
-                           password='1',
-                           database='test_base',
-                           charset='utf8',
-                           cursorclass=pymysql.cursors.DictCursor)
-    return conn
-def close_db_connection(conn):
-    conn.close()
-@app.route("/")
-def index():
-    conn = get_db_connection()
-    with conn.cursor() as cur:
-        cur.execute("SELECT * FROM test_table")
-        test_list_posts = cur.fetchall()
-    conn.close()
-    page, per_page, offset = get_page_args(page_parameter='page',
-                                           per_page_parameter='per_page')
-    total = len(test_list_posts)
-    def get_test_list_posts(offset=0, per_page=5):
-        return test_list_posts[offset: offset + per_page]
-    pagination_test_list_posts = get_test_list_posts(offset=offset, per_page=per_page)
-    pagination = Pagination(page=page, per_page=per_page, total=total,
-                        css_framework='bootstrap4',
-                        display_msg="Показано &lt;b&gt;{start} - {end}&lt;/b&gt; {record_name} из &lt;b&gt;{total}&lt;/b&gt;",
-                        record_name="записей")
-    return flask.render_template("test/test_list_posts.html",
-                                 test_list_posts=pagination_test_list_posts, 
-                                                            page=page,
-                           per_page=per_page,
-                           pagination=pagination,)
-@app.route("/view/&lt;int:test_id&gt;")
-def get_post_test_post(test_id):
-    conn = get_db_connection()
-    with conn.cursor() as cur:
-        sql = "SELECT * FROM `test_table` WHERE `test_id` =%s"
-        cur.execute(sql, test_id)
-        test_view_post = cur.fetchone()
-    conn.close()
-    return flask.render_template("test/test_view_post.html",
-                                 test_view_post=test_view_post, )
-@app.route("/edit/&lt;int:test_id&gt;/", methods=("GET", "POST"))
-def edit_test_post(test_id):
-    conn = get_db_connection()
-    with conn.cursor() as cur:
-        sql = "SELECT * FROM `test_table` WHERE `test_id` =%s"
-        cur.execute(sql, (test_id,))
-        edit_test_view = cur.fetchone()
-    if flask.request.method == "POST":
-        test_edit_post_text = flask.request.form["test_text"]
-        if len(flask.request.form['test_text']) &gt; 1:
-            conn = get_db_connection()
-            with conn.cursor() as cur:
-                sql = "UPDATE `test_table` SET `test_text` =%s  WHERE `test_id` =%s"
-                cur.execute(
-                    sql, (test_edit_post_text, test_id),
-                )
-            conn.commit()
-            conn.close()
-            if not test_edit_post_text:
-                flask.flash('Ошибка сохранения записи, вы ввели мало символов!', category='error')
-            else:
-                flask.flash('Запись успешно сохранена!', category='success')
-            # В случае соблюдения условий заполнения полей, произойдёт перенаправление
-            return flask.redirect(flask.url_for("index"))
-        else:
-            flask.flash('Ошибка сохранения записи!', category='error')
-    return flask.render_template("test/edit_test_post.html", edit_test_view=edit_test_view)
-@app.route("/new_post", methods=["GET", "POST"])
-def add_test_post():
-    if flask.request.method == "POST":
-        new_test_post = flask.request.form["test_text"]
-        if len(flask.request.form['test_text']) &gt; 1:
-            conn = get_db_connection()
-            with conn.cursor() as cur:
-                sql = "INSERT INTO `test_table` (`test_text`) VALUES (%s)"
-                cur.execute(
-                    sql, new_test_post,
-                )
-            conn.commit()
-            conn.close()
-            if not new_test_post:
-                flask.flash('Ошибка сохранения записи, Вы ввели слишком мало символов!', category='error')
-            else:
-                flask.flash('Запись успешно добавлена!')
-            # В случае соблюдения условий заполнения полей, произойдёт перенаправление
-            return flask.redirect(flask.url_for("index"))
-        else:
-            flask.flash('Ошибка сохранения записи!', category='error')
-    return flask.render_template("test/add_test_post.html")
-@app.route("/delete/&lt;int:test_id&gt;/", methods=("POST",))
-def delete_post_test(test_id):
-    conn = get_db_connection()
-    with conn.cursor() as cur:
-        sql = "DELETE FROM `test_table` WHERE `test_id` =%s"
-        cur.execute(
-            sql, test_id,
-        )
-    conn.commit()
-    conn.close()
-    return flask.redirect(flask.url_for("index"))
-if __name__ == "__main__":
-    app.run(debug=True, host='0.0.0.0', port=83)</t>
         </is>
       </c>
     </row>
@@ -1470,7 +1150,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1480,156 +1160,156 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Поисковая система Google</t>
+          <t>Что такое CLI?</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>google.com</t>
+          <t>ru.wikipedia.org/wiki/Интерфейс_командной_строки</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Поисковая система Google</t>
+          <t>Что такое CLI?</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Яндекс</t>
+          <t>Blueprint</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>yandex.ru</t>
+          <t>dnmtechs.com/splitting-a-python-flask-app-into-multiple-files/</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Поисковая система</t>
+          <t>Разбивка приложения на части</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Blueprint</t>
+          <t>Документация CLI PowerSHell</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>dnmtechs.com/splitting-a-python-flask-app-into-multiple-files/</t>
+          <t>learn.microsoft.com/ru-ru/powershell/</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Разбивка приложения на части</t>
+          <t>Документация CLI PowerSHell</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Документация CLI PowerSHell</t>
+          <t>Описание библиотеки, которая позволяет работает с базой mysql</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>learn.microsoft.com/ru-ru/powershell/</t>
+          <t>pypi.org/project/PyMySQL/</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Документация CLI PowerSHell</t>
+          <t>Описание библиотеки, которая позволяет работает с базой mysql.</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Описание библиотеки, которая позволяет работает с базой mysql</t>
+          <t>Документация по Bootstrap</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>pypi.org/project/PyMySQL/</t>
+          <t>getbootstrap.com/</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Описание библиотеки, которая позволяет работает с базой mysql.</t>
+          <t>Документация по Bootstrap.</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Документация по Bootstrap</t>
+          <t>Сайт с документацией по веб-технологиям</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>getbootstrap.com/</t>
+          <t>developer.mozilla.org/ru/docs/Web</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Документация по Bootstrap.</t>
+          <t>Сайт с документацией по веб-технологиям.</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Сайт с документацией по веб-технологиям</t>
+          <t>Работа с gitignore</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>developer.mozilla.org/ru/docs/Web</t>
+          <t>wiki.merionet.ru/articles/fajl-gitignore-kak-ignorirovat-fajly-i-papki-v-git</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Сайт с документацией по веб-технологиям.</t>
+          <t>None</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Работа с gitignore</t>
+          <t>Красивый python</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>wiki.merionet.ru/articles/fajl-gitignore-kak-ignorirovat-fajly-i-papki-v-git</t>
+          <t>sky.pro/media/pep8/</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -1640,16 +1320,16 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Красивый python</t>
+          <t>Горячие клавиши Bash</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>sky.pro/media/pep8/</t>
+          <t>selectel.ru/blog/tutorials/linux-terminal-hotkeys/</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -1660,16 +1340,16 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Горячие клавиши Bash</t>
+          <t>Интересный материал про bash</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>selectel.ru/blog/tutorials/linux-terminal-hotkeys/</t>
+          <t>linuxsimply.com/bash-scripting-tutorial/basics/</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1680,16 +1360,16 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Интересный материал про bash</t>
+          <t>Список команд Windows CMD с описанием и примерами</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>linuxsimply.com/bash-scripting-tutorial/basics/</t>
+          <t>ab57.ru/cmdlist.html</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1700,16 +1380,16 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Список команд Windows CMD с описанием и примерами</t>
+          <t>Работа с 7zip из командной строки</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>ab57.ru/cmdlist.html</t>
+          <t xml:space="preserve">dmosk.ru/miniinstruktions.php?mini=7zip-cmd </t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1720,16 +1400,16 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Работа с 7zip из командной строки</t>
+          <t>Как создать и запустить bat-файлы</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t xml:space="preserve">dmosk.ru/miniinstruktions.php?mini=7zip-cmd </t>
+          <t>nic.ru/help/kak-sozdat6-i-zapustit6-bat-fajly_11640.html</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1740,39 +1420,19 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Как создать и запустить bat-файлы</t>
+          <t>Как сделать скрипт на bash</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>nic.ru/help/kak-sozdat6-i-zapustit6-bat-fajly_11640.html</t>
+          <t>selectel.ru/blog/tutorials/linux-bash-scripting-guide/</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>1</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Как сделать скрипт на bash</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>selectel.ru/blog/tutorials/linux-bash-scripting-guide/</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -2924,7 +2584,7 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Перенос файла в другой диск</t>
+          <t>Перенос файла на другой диск</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Hotfix: Sat Nov  2 14:54:45 RTZ 2024
</commit_message>
<xml_diff>
--- a/files/database_tables.xlsx
+++ b/files/database_tables.xlsx
@@ -635,7 +635,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1307,6 +1307,21 @@
         </is>
       </c>
     </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>2110</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>dfgfdgfd</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>gdfgfdgfdgdfggfd</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Hotfix: Tue Nov  5 14:57:49 RTZ 2024
</commit_message>
<xml_diff>
--- a/files/database_tables.xlsx
+++ b/files/database_tables.xlsx
@@ -635,7 +635,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1307,21 +1307,6 @@
         </is>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" t="n">
-        <v>2110</v>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>dfgfdgfd</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>gdfgfdgfdgdfggfd</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1333,7 +1318,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1343,106 +1328,106 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Grid сетка</t>
+          <t>Как сделать скрипт на bash</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>skillbox.ru/media/code/uchimsya-verstat-v-setke-bolshoy-gayd-po-css-grid/</t>
+          <t>https://selectel.ru/blog/tutorials/linux-bash-scripting-guide/</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Что такое CLI?</t>
+          <t>Как создать и запустить bat-файлы</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ru.wikipedia.org/wiki/Интерфейс_командной_строки</t>
+          <t>https://nic.ru/help/kak-sozdat6-i-zapustit6-bat-fajly_11640.html</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Blueprint</t>
+          <t>Работа с 7zip из командной строки</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>dnmtechs.com/splitting-a-python-flask-app-into-multiple-files/</t>
+          <t xml:space="preserve">https://dmosk.ru/miniinstruktions.php?mini=7zip-cmd </t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Документация CLI PowerSHell</t>
+          <t>Список команд Windows CMD с описанием и примерами</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>learn.microsoft.com/ru-ru/powershell/</t>
+          <t>https://ab57.ru/cmdlist.html</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Описание библиотеки, которая позволяет работает с базой mysql</t>
+          <t>Интересный материал про bash</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>pypi.org/project/PyMySQL/</t>
+          <t>https://linuxsimply.com/bash-scripting-tutorial/basics/</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Документация по Bootstrap</t>
+          <t>Горячие клавиши Bash</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>getbootstrap.com/</t>
+          <t>https://selectel.ru/blog/tutorials/linux-terminal-hotkeys/</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Сайт с документацией по веб-технологиям</t>
+          <t>Красивый python</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>developer.mozilla.org/ru/docs/Web</t>
+          <t>https://sky.pro/media/pep8/</t>
         </is>
       </c>
     </row>
@@ -1457,112 +1442,127 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>wiki.merionet.ru/articles/fajl-gitignore-kak-ignorirovat-fajly-i-papki-v-git</t>
+          <t>https://wiki.merionet.ru/articles/fajl-gitignore-kak-ignorirovat-fajly-i-papki-v-git</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Красивый python</t>
+          <t>Сайт с документацией по веб-технологиям</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>sky.pro/media/pep8/</t>
+          <t>https://developer.mozilla.org/ru/docs/Web</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Горячие клавиши Bash</t>
+          <t>Документация по Bootstrap</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>selectel.ru/blog/tutorials/linux-terminal-hotkeys/</t>
+          <t>https://getbootstrap.com/</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Интересный материал про bash</t>
+          <t>Описание библиотеки, которая позволяет работает с базой mysql</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>linuxsimply.com/bash-scripting-tutorial/basics/</t>
+          <t>https://pypi.org/project/PyMySQL/</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Список команд Windows CMD с описанием и примерами</t>
+          <t>Документация CLI PowerSHell</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>ab57.ru/cmdlist.html</t>
+          <t>https://learn.microsoft.com/ru-ru/powershell/</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Работа с 7zip из командной строки</t>
+          <t>Blueprint</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t xml:space="preserve">dmosk.ru/miniinstruktions.php?mini=7zip-cmd </t>
+          <t>https://dnmtechs.com/splitting-a-python-flask-app-into-multiple-files/</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Как создать и запустить bat-файлы</t>
+          <t>Что такое CLI?</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>nic.ru/help/kak-sozdat6-i-zapustit6-bat-fajly_11640.html</t>
+          <t>https://ru.wikipedia.org/wiki/Интерфейс_командной_строки</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Как сделать скрипт на bash</t>
+          <t>Grid сетка</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>selectel.ru/blog/tutorials/linux-bash-scripting-guide/</t>
+          <t>https://skillbox.ru/media/code/uchimsya-verstat-v-setke-bolshoy-gayd-po-css-grid/</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>51</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Полезная страница с методами работы с файлами в Python.</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>https://victor-komlev.ru/rabota-s-operatsionnoj-i-fajlovoj-sistemoj-v-python-pathlib-os-shutil/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Hotfix: Thu Nov  7 17:45:45 RTZ 2024
</commit_message>
<xml_diff>
--- a/files/database_tables.xlsx
+++ b/files/database_tables.xlsx
@@ -1318,7 +1318,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1563,6 +1563,22 @@
       <c r="C16" t="inlineStr">
         <is>
           <t>https://victor-komlev.ru/rabota-s-operatsionnoj-i-fajlovoj-sistemoj-v-python-pathlib-os-shutil/</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>52</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Ссылка на очень удобную программу Samsung Dex. 
+Программа предназначена на для трансляции экрана телефона Samsung на ПК.</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>https://www.samsung.com/ru/apps/samsung-dex/</t>
         </is>
       </c>
     </row>
@@ -1577,7 +1593,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C75"/>
+  <dimension ref="A1:C80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2743,6 +2759,83 @@
         </is>
       </c>
     </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>129</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>~/AppData/Local/Programs/Python/Python313/python.exe -m webbrowser http://127.0.0.1:82</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Запуск приложения в браузере</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>130</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Set-ExecutionPolicy RemoteSigned</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Разрешение запуска сценариев powershell</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>131</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>where powershell</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Как найти исполняемый файл powershell в системе?
+Ввести в cmd команду!</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>132</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>python -m pip uninstall -r requirements.txt -y</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Принудительное деинсталляция пакетов из файла requirements.txt </t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>133</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>#!/c/Windows/System32/WindowsPowerShell/v1.0/powershell.exe
+Stop-Process -Name "python"</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Скрипт powershell, который убивает все python запущенные процессы</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Hotfix: Thu Nov 14 11:24:26 RTZ 2024
</commit_message>
<xml_diff>
--- a/files/database_tables.xlsx
+++ b/files/database_tables.xlsx
@@ -2850,7 +2850,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2880,6 +2880,37 @@
         </is>
       </c>
       <c r="E1" t="inlineStr">
+        <is>
+          <t>Опубликован</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>4</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Бэкэнд-фиксы</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>3.7</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - Поправлен скрипт запуска приложения.
+Теперь приложение запуститься в браузере через 5 секунд только при наличии интернета.
+ - Дописан файл readme.md
+ - Создан отдельный файл imports.py
+В него из файла app.py перенесены все импортирумые модули приложения.
+Сделано это для разгрузки файла запуска скрипта основного приложения.
+ - Из app.py перенесена логика проверки файла базы данных в модуль connect.py</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
         <is>
           <t>Опубликован</t>
         </is>

</xml_diff>

<commit_message>
Hotfix: Fri Nov 15 11:48:48 RTZ 2024
</commit_message>
<xml_diff>
--- a/files/database_tables.xlsx
+++ b/files/database_tables.xlsx
@@ -9,11 +9,10 @@
   <sheets>
     <sheet name="SQL" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Python" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Links" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="HTML" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Bash" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Releases" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Tasks" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Test" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="CSS" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Test" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -638,7 +637,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1310,6 +1309,72 @@
         </is>
       </c>
     </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>2111</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">UPLOAD_FOLDER = 'static'
+# расширения файлов, которые разрешено загружать
+ALLOWED_EXTENSIONS = {'txt', 'pdf', 'png', 'jpg', 'jpeg', 'gif'}
+# конфигурируем
+app.config['UPLOAD_FOLDER'] = UPLOAD_FOLDER
+app.secret_key = "secret key"
+@app.route("/upload")
+def upload_images():
+    return render_template("upload.html")
+@app.route('/', methods=['POST'])
+def upload_file():
+    if request.method == 'POST':
+        # check if the post request has the file part
+        if 'file' not in request.files:
+            flash('No file part')
+            return redirect(request.url)
+        file = request.files['file']
+        if file.filename == '':
+            flash('No file selected for uploading')
+            return redirect(request.url)
+        if file and allowed_file(file.filename):
+            filename = secure_filename(file.filename)
+            file.save(os.path.join(app.config['UPLOAD_FOLDER'], filename))
+            flash('File successfully uploaded')
+            return redirect('/upload')
+        else:
+            flash('Allowed file types are txt, pdf, png, jpg, jpeg, gif, py, docx')
+            return redirect(request.url)
+&lt;title&gt;Python Flask File Upload Example&lt;/title&gt;
+&lt;h2&gt;Select a file to upload&lt;/h4&gt;
+&lt;p&gt;
+   {% with messages = get_flashed_messages() %}
+     {% if messages %}
+      &lt;ul class=flashes&gt;
+      {% for message in messages %}
+        &lt;li&gt;{{ message }}&lt;/li&gt;
+      {% endfor %}
+      &lt;/ul&gt;
+     {% endif %}
+   {% endwith %}
+&lt;/p&gt;
+&lt;form method="post" action="/" enctype="multipart/form-data"&gt;
+    &lt;dl&gt;
+      &lt;p&gt;
+         &lt;input type="file" name="file" autocomplete="off" required&gt;
+      &lt;/p&gt;
+    &lt;/dl&gt;
+    &lt;p&gt;
+      &lt;input type="submit" value="Submit"&gt;
+   &lt;/p&gt;
+&lt;/form&gt;
+</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Логика и представление загрузки картинки в приложение</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1321,7 +1386,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1335,255 +1400,20 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Как сделать скрипт на bash</t>
+          <t>test</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>https://selectel.ru/blog/tutorials/linux-bash-scripting-guide/</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Как создать и запустить bat-файлы</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>https://nic.ru/help/kak-sozdat6-i-zapustit6-bat-fajly_11640.html</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>3</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Работа с 7zip из командной строки</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">https://dmosk.ru/miniinstruktions.php?mini=7zip-cmd </t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>4</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Список команд Windows CMD с описанием и примерами</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>https://ab57.ru/cmdlist.html</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>5</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Интересный материал про bash</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>https://linuxsimply.com/bash-scripting-tutorial/basics/</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>15</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Горячие клавиши Bash</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>https://selectel.ru/blog/tutorials/linux-terminal-hotkeys/</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>16</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Красивый python</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>https://sky.pro/media/pep8/</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>17</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Работа с gitignore</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>https://wiki.merionet.ru/articles/fajl-gitignore-kak-ignorirovat-fajly-i-papki-v-git</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>19</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Сайт с документацией по веб-технологиям</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>https://developer.mozilla.org/ru/docs/Web</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>20</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Документация по Bootstrap</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>https://getbootstrap.com/</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>21</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Описание библиотеки, которая позволяет работает с базой mysql</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>https://pypi.org/project/PyMySQL/</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>22</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Документация CLI PowerSHell</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>https://learn.microsoft.com/ru-ru/powershell/</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>25</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Blueprint</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>https://dnmtechs.com/splitting-a-python-flask-app-into-multiple-files/</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>33</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Что такое CLI?</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>https://ru.wikipedia.org/wiki/Интерфейс_командной_строки</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>50</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Grid сетка</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>https://skillbox.ru/media/code/uchimsya-verstat-v-setke-bolshoy-gayd-po-css-grid/</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>51</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Полезная страница с методами работы с файлами в Python.</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>https://victor-komlev.ru/rabota-s-operatsionnoj-i-fajlovoj-sistemoj-v-python-pathlib-os-shutil/</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>52</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Ссылка на очень удобную программу Samsung Dex. 
-Программа предназначена на для трансляции экрана телефона Samsung на ПК.</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>https://www.samsung.com/ru/apps/samsung-dex/</t>
-        </is>
-      </c>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>2024-11-13 08:40:02</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1596,7 +1426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C80"/>
+  <dimension ref="A1:C81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2360,7 +2190,10 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>~/AppData/Local/Programs/Python/Python312/python.exe venv/Scripts/pip.exe install -r requirements.txt</t>
+          <t>Вариант использования с виртуальным окружением:
+~/AppData/Local/Programs/Python/Python312/python.exe venv/Scripts/pip.exe install -r requirements.txt
+Вариант использования установленным систему PATH:
+pip install -r requirements.txt</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2839,6 +2672,21 @@
         </is>
       </c>
     </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>134</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>pip install --upgrade -r requirements.txt</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Проверка обновлений библиотек</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -2850,7 +2698,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2860,61 +2708,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Релизы</t>
+          <t>test</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>test</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> - Добавлен раздел "Релизы" на проект;
- - Во все скрипты создания дампа и создания таблиц занесены все разделы;
-</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Опубликован</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>4</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Бэкэнд-фиксы</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>3.7</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> - Поправлен скрипт запуска приложения.
-Теперь приложение запуститься в браузере через 5 секунд только при наличии интернета.
- - Дописан файл readme.md
- - Создан отдельный файл imports.py
-В него из файла app.py перенесены все импортирумые модули приложения.
-Сделано это для разгрузки файла запуска скрипта основного приложения.
- - Из app.py перенесена логика проверки файла базы данных в модуль connect.py</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Опубликован</t>
-        </is>
-      </c>
+          <t>2024-11-13 10:58:04</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2922,24 +2733,6 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
Hotfix: Fri Nov 15 16:22:21 RTZ 2024
</commit_message>
<xml_diff>
--- a/files/database_tables.xlsx
+++ b/files/database_tables.xlsx
@@ -637,7 +637,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -659,6 +659,12 @@
           <t>Выводит тип данных</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:09:33</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr"/>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -674,6 +680,12 @@
           <t>Экспорт в формат CSV</t>
         </is>
       </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:09:33</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -689,6 +701,12 @@
           <t>Копирование датафрейма</t>
         </is>
       </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:09:33</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -704,6 +722,12 @@
           <t>Подсчёт количества строк в датафрейме</t>
         </is>
       </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:09:33</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -719,6 +743,12 @@
           <t>Подсчёт количества уникальных значений в столбце</t>
         </is>
       </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:09:33</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -734,6 +764,12 @@
           <t>Вывод статистических сведений о датафрейме</t>
         </is>
       </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:09:33</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -749,6 +785,12 @@
           <t>Для того чтобы подсчитать количество значений в конкретном столбце, можно воспользоваться следующей конструкцие</t>
         </is>
       </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:09:33</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -764,6 +806,12 @@
           <t>Получение списка значений столбцов</t>
         </is>
       </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:09:33</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -779,6 +827,12 @@
           <t>Создание списка или объекта Series на основе значений столбца</t>
         </is>
       </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:09:33</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -794,6 +848,12 @@
           <t>Присоединение к датафрейму нового столбца с заданным значением</t>
         </is>
       </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:09:33</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -809,6 +869,12 @@
           <t>Создание нового датафрейма из подмножества столбцов</t>
         </is>
       </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:09:33</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -824,6 +890,12 @@
           <t>Удаление столбца</t>
         </is>
       </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:09:33</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -839,6 +911,12 @@
           <t>Получение строк по числовым индексам</t>
         </is>
       </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:09:33</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -854,6 +932,12 @@
           <t>Для получения строк датафрейма в ситуации, когда имеется список значений столбцов, можно воспользоваться следующей командой</t>
         </is>
       </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:09:33</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -869,6 +953,12 @@
           <t>Фильтрация по значению</t>
         </is>
       </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:09:33</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -884,6 +974,12 @@
           <t>Сортировка</t>
         </is>
       </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:09:33</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -899,6 +995,12 @@
           <t>Функция df.groupby и подсчёт количества записей</t>
         </is>
       </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:09:33</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -914,6 +1016,12 @@
           <t>Получение строк с нужными индексными значениями</t>
         </is>
       </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:09:33</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -929,6 +1037,12 @@
           <t>Слияние датафреймов</t>
         </is>
       </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:09:33</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -944,6 +1058,12 @@
           <t>Получение сведений о датафрейм</t>
         </is>
       </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:09:33</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -959,6 +1079,12 @@
           <t>Вывести первые пять строк датасета</t>
         </is>
       </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:09:33</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -974,6 +1100,12 @@
           <t>Удаление нескольких столбцов</t>
         </is>
       </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:09:33</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -989,6 +1121,12 @@
           <t>Переименование столбца</t>
         </is>
       </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:09:33</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -1004,6 +1142,12 @@
           <t>Вывести количество строк и столбцов датасета</t>
         </is>
       </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:09:33</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -1019,6 +1163,12 @@
           <t>Получим максимальные значения в каждом столбце</t>
         </is>
       </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:09:33</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -1034,6 +1184,12 @@
           <t>Изменение типа столбца</t>
         </is>
       </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:09:33</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -1049,6 +1205,12 @@
           <t>Создание датафрейма из базы данных</t>
         </is>
       </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:09:33</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -1064,6 +1226,12 @@
           <t>Загрузка данных из EXCEL файла</t>
         </is>
       </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:09:33</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -1079,6 +1247,12 @@
           <t>Загрузка CSV-данных в датафрейм</t>
         </is>
       </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:09:33</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -1206,6 +1380,12 @@
           <t>Экземляр app.py mysql connect</t>
         </is>
       </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:09:33</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -1227,6 +1407,12 @@
           <t>Преобразование данных таблицы в датафрейм</t>
         </is>
       </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:09:33</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -1263,6 +1449,12 @@
           <t>Создание таблицы в базе данных</t>
         </is>
       </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:09:33</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -1282,6 +1474,12 @@
           <t>Удаление таблицы в базе данных</t>
         </is>
       </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:09:33</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -1308,6 +1506,12 @@
           <t>Вставка значений в таблицу базы данных</t>
         </is>
       </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:09:33</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -1374,6 +1578,35 @@
           <t>Логика и представление загрузки картинки в приложение</t>
         </is>
       </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:09:33</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>2116</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>import datetime
+dt_now = datetime.datetime.now()
+print(dt_now)</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Вывод текущей латы и времени</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:09:33</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1386,36 +1619,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>2024-11-13 08:40:02</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr"/>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -2698,7 +2909,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2708,24 +2919,56 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>Первая запись в CSS11</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>Первая запись в CSS11</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>2024-11-13 10:58:04</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr"/>
+          <t>2024-11-15 10:41:09</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>2024-11-15 14:16:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>4</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Свойство border-radius</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>/* Свойство задает округление элементу HTML */
+border-radius: 10px;
+/* top-left-and-bottom-right | top-right-and-bottom-left */
+border-radius: 10px 5%;
+/* top-left | top-right-and-bottom-left | bottom-right */
+border-radius: 2px 4px 2px;
+/* top-left | top-right | bottom-right | bottom-left */
+border-radius: 1px 0 3px 4px;</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2024-11-15 11:23:21</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Hotfix: Fri Nov 15 16:48:15 RTZ 2024
</commit_message>
<xml_diff>
--- a/files/database_tables.xlsx
+++ b/files/database_tables.xlsx
@@ -1637,7 +1637,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C81"/>
+  <dimension ref="A1:E81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1659,6 +1659,12 @@
           <t>Удаление последней набранной строки</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr"/>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -1674,6 +1680,12 @@
           <t>Поиск текста в истории</t>
         </is>
       </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -1689,6 +1701,12 @@
           <t>Копирование файлов</t>
         </is>
       </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -1704,6 +1722,12 @@
           <t>Очистка экрана</t>
         </is>
       </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -1719,6 +1743,12 @@
           <t>Завершает процесс</t>
         </is>
       </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -1734,6 +1764,12 @@
           <t>История команд</t>
         </is>
       </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -1749,6 +1785,12 @@
           <t>Выводит список процессов</t>
         </is>
       </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1764,6 +1806,12 @@
           <t>Показывает текущий путь к папке</t>
         </is>
       </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1779,6 +1827,12 @@
           <t>Возврат в вышестоящую директорию</t>
         </is>
       </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1794,6 +1848,12 @@
           <t>Возврат на две папки выше</t>
         </is>
       </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1809,6 +1869,12 @@
           <t>Переход в корневую папку</t>
         </is>
       </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1824,6 +1890,12 @@
           <t>Вывод содержимого каталога(файлов и папок)</t>
         </is>
       </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1839,6 +1911,12 @@
           <t>Вернуться назад</t>
         </is>
       </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1854,6 +1932,12 @@
           <t>Переход  в оперделенную папку</t>
         </is>
       </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1869,6 +1953,12 @@
           <t>Показать файлы в данной папке, включая и скрытые</t>
         </is>
       </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1884,6 +1974,12 @@
           <t>Вывод папок раздела</t>
         </is>
       </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1899,6 +1995,12 @@
           <t>Создание папки или папок(несколько папок через пробел нужно указать)</t>
         </is>
       </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1914,6 +2016,12 @@
           <t>Файл intro перенесется в папку manual под именем chap1</t>
         </is>
       </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -1929,6 +2037,12 @@
           <t>Файл chap3 перенесется в папку manual</t>
         </is>
       </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1944,6 +2058,12 @@
           <t>Файл appendix переименуется в apndx.a</t>
         </is>
       </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1959,6 +2079,12 @@
           <t>Чтение указанного файла</t>
         </is>
       </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -1974,6 +2100,12 @@
           <t>Удаление файла</t>
         </is>
       </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -1989,6 +2121,12 @@
           <t>Удаление папки с содержанием</t>
         </is>
       </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -2004,6 +2142,12 @@
           <t>Удаление папки с содержанием принудительно</t>
         </is>
       </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -2019,6 +2163,12 @@
           <t>Выход из командной строки</t>
         </is>
       </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -2034,6 +2184,12 @@
           <t>Запрос DNS определенного адреса</t>
         </is>
       </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -2049,6 +2205,12 @@
           <t>Запуск процесса в фоновом режиме</t>
         </is>
       </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -2064,6 +2226,12 @@
           <t>Генерация ssh-ключа</t>
         </is>
       </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -2079,6 +2247,12 @@
           <t>Создание виртуального окружения Python</t>
         </is>
       </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -2094,6 +2268,12 @@
           <t>Создание файла скрипта bash.sh</t>
         </is>
       </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -2109,6 +2289,12 @@
           <t>Открытие файла встроенным bash редактором</t>
         </is>
       </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -2124,6 +2310,12 @@
           <t>Запуск скрипта bash</t>
         </is>
       </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -2139,6 +2331,12 @@
           <t>Настройка прав на файл скрипта</t>
         </is>
       </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -2154,6 +2352,12 @@
           <t>Выводит списокм папки и файлы текущего раздела с датой изменения, размером и правами доступа</t>
         </is>
       </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -2169,6 +2373,12 @@
           <t>Удаляет все файлы в текущей директории</t>
         </is>
       </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -2184,6 +2394,12 @@
           <t>Удаляет все команды из истории</t>
         </is>
       </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -2199,6 +2415,12 @@
           <t>Вывод текущей даты и времени</t>
         </is>
       </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -2214,6 +2436,12 @@
           <t>Создаем две папки в текущем каталоге</t>
         </is>
       </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -2229,6 +2457,12 @@
           <t>Удаление всех папок текущей директории</t>
         </is>
       </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -2244,6 +2478,12 @@
           <t>Установки нужной библиотеки</t>
         </is>
       </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -2259,6 +2499,12 @@
           <t>Переход из текущего раздела в другой раздел с определенной папкой</t>
         </is>
       </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -2274,6 +2520,12 @@
           <t>Выводит на экран все файлы с указанным расширением</t>
         </is>
       </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -2289,6 +2541,12 @@
           <t>Вернуться в корневую папку</t>
         </is>
       </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -2304,6 +2562,12 @@
           <t>Копирование всех файлов в другую папку</t>
         </is>
       </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -2319,6 +2583,12 @@
           <t>Поиск процесса по имени</t>
         </is>
       </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -2334,6 +2604,12 @@
           <t>Завершить работы всех приложений python</t>
         </is>
       </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -2349,6 +2625,12 @@
           <t>Вывод всех процессов Windows по имени</t>
         </is>
       </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -2364,6 +2646,12 @@
           <t>Остановка процессов по имени</t>
         </is>
       </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -2379,6 +2667,12 @@
           <t>Удаление папки с файлами в PowerShell</t>
         </is>
       </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -2394,6 +2688,12 @@
           <t>Создание файла с пакетами</t>
         </is>
       </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -2412,6 +2712,12 @@
           <t>Устанавливает из файла все пакеты</t>
         </is>
       </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -2427,6 +2733,12 @@
           <t>Перемещение файла из текущей папки в вышестоящий раздел</t>
         </is>
       </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -2442,6 +2754,12 @@
           <t>Перемещение нескольких файлов в другую папку с определенным расширением</t>
         </is>
       </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -2457,6 +2775,12 @@
           <t>Запуск bash скрипта из любой директории</t>
         </is>
       </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -2472,6 +2796,12 @@
           <t>Назначение git глобальной почты</t>
         </is>
       </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -2487,6 +2817,12 @@
           <t>Назначение git глобального имени</t>
         </is>
       </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -2502,6 +2838,12 @@
           <t>Клонирование удаленного репозитория</t>
         </is>
       </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -2517,6 +2859,12 @@
           <t>Статус изменений</t>
         </is>
       </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="n">
@@ -2532,6 +2880,12 @@
           <t>Вывод конфигурации git</t>
         </is>
       </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -2547,6 +2901,12 @@
           <t>Подготовка файлов для коммита</t>
         </is>
       </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -2562,6 +2922,12 @@
           <t>Подготовка коммита</t>
         </is>
       </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -2577,6 +2943,12 @@
           <t>Отправка изменений на репозиторий</t>
         </is>
       </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="n">
@@ -2592,6 +2964,12 @@
           <t>Инициализация git в папке</t>
         </is>
       </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -2607,6 +2985,12 @@
           <t>Скачивание изменения из репозитория на локальную машину</t>
         </is>
       </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="n">
@@ -2622,6 +3006,12 @@
           <t>Обновление pip</t>
         </is>
       </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -2637,6 +3027,12 @@
           <t>Установка библиотеки Pandas</t>
         </is>
       </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="n">
@@ -2655,6 +3051,12 @@
 </t>
         </is>
       </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="n">
@@ -2681,6 +3083,12 @@
 </t>
         </is>
       </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="n">
@@ -2703,6 +3111,12 @@
 </t>
         </is>
       </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -2718,6 +3132,12 @@
           <t>Переименование файла в CMD</t>
         </is>
       </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="n">
@@ -2733,6 +3153,12 @@
           <t>Вывод всех подключенных дисков</t>
         </is>
       </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="n">
@@ -2748,6 +3174,12 @@
           <t>Скрипт архивации файлов и перенос архива на другой диск</t>
         </is>
       </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="n">
@@ -2763,6 +3195,12 @@
           <t>Создание архива всех файлов в папке</t>
         </is>
       </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="n">
@@ -2778,6 +3216,12 @@
           <t>Перенос файла на другой диск</t>
         </is>
       </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="n">
@@ -2805,6 +3249,12 @@
           <t>Скрипт отправляет на репозиторий коммит с указанием номера релиза(cli спрашивает у юзера), делает архив проекта и отправляет на другой диск</t>
         </is>
       </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="n">
@@ -2820,6 +3270,12 @@
           <t>Запуск приложения в браузере</t>
         </is>
       </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="n">
@@ -2835,6 +3291,12 @@
           <t>Разрешение запуска сценариев powershell</t>
         </is>
       </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="n">
@@ -2851,6 +3313,12 @@
 Ввести в cmd команду!</t>
         </is>
       </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="n">
@@ -2866,6 +3334,12 @@
           <t xml:space="preserve">Принудительное деинсталляция пакетов из файла requirements.txt </t>
         </is>
       </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="n">
@@ -2882,6 +3356,12 @@
           <t>Скрипт powershell, который убивает все python запущенные процессы</t>
         </is>
       </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="n">
@@ -2897,6 +3377,12 @@
           <t>Проверка обновлений библиотек</t>
         </is>
       </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>2024-11-15 13:18:16</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Hotfix: Tue Nov 19 17:53:55 RTZ 2024
</commit_message>
<xml_diff>
--- a/files/database_tables.xlsx
+++ b/files/database_tables.xlsx
@@ -418,7 +418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -432,14 +432,20 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>Добавление новой записи в таблицу</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
           <t>INSERT INTO git_and_bash (command, name) VALUES ('test', 'test')</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Добавление новой записи в таблицу</t>
-        </is>
-      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>2024-11-19 13:58:50</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr"/>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -447,14 +453,20 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>Поиск в поле значений по части слова</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>SELECT * FROM git_and_bash WHERE command LIKE '%ls%'</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Поиск в поле значений по части слова</t>
-        </is>
-      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2024-11-19 13:58:50</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -462,14 +474,20 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>Сортировка всех записей по убыванию</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>SELECT * FROM links ORDER BY id DESC</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Сортировка всех записей по убыванию</t>
-        </is>
-      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2024-11-19 13:58:50</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -477,14 +495,20 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>Сортировка по возрастанию</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>SELECT * FROM links ORDER BY id ASC</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Сортировка по возрастанию</t>
-        </is>
-      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2024-11-19 13:58:50</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -492,14 +516,20 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>Удаление определенной записи</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
           <t>DELETE FROM git_and_bash WHERE id = 45</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Удаление определенной записи</t>
-        </is>
-      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2024-11-19 13:58:50</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -507,14 +537,20 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>Очистка таблицы</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
           <t>DELETE FROM [train];</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Очистка таблицы</t>
-        </is>
-      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2024-11-19 13:58:50</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -522,14 +558,20 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>Изменение значения записи определенного поля</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
           <t>UPDATE [sql] SET [name]='Сортировка всех записей по убыванию' WHERE ([sql].[id] = 3);</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Изменение значения записи определенного поля</t>
-        </is>
-      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2024-11-19 13:58:50</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -537,14 +579,20 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>Добавление поля в таблицу</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
           <t>ALTER TABLE [train] ADD [imya] VARCHAR(250) NOT NULL;</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Добавление поля в таблицу</t>
-        </is>
-      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2024-11-19 13:58:50</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -552,14 +600,20 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
+          <t>Переименование поля таблицы</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
           <t>ALTER TABLE [train] RENAME COLUMN [train_name] TO [familia];</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Переименование поля таблицы</t>
-        </is>
-      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2024-11-19 13:58:50</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -567,14 +621,20 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>Удаляет таблицу базы данных</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
           <t>DROP TABLE [train];</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Удаляет таблицу базы данных</t>
-        </is>
-      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2024-11-19 13:58:50</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -582,14 +642,20 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
+          <t>Поиск уникальных значений</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
           <t>SELECT DISTINCT field FROM table;</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Поиск уникальных значений</t>
-        </is>
-      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2024-11-19 13:58:50</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -597,20 +663,31 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>Вывод всех записей таблицы</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
           <t>SELECT * FROM table;</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Вывод всех записей таблицы</t>
-        </is>
-      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>2024-11-19 13:58:50</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
         <v>1167</v>
       </c>
       <c r="B13" t="inlineStr">
+        <is>
+          <t>Создание таблицы в базе данных</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
         <is>
           <t>CREATE TABLE IF NOT EXISTS tasks (
   task_id INTEGER PRIMARY KEY AUTOINCREMENT,
@@ -620,11 +697,12 @@
 );</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Создание таблицы в базе данных</t>
-        </is>
-      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2024-11-19 13:58:50</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Hotfix: Wed Nov 20 17:48:22 RTZ 2024
</commit_message>
<xml_diff>
--- a/files/database_tables.xlsx
+++ b/files/database_tables.xlsx
@@ -684,7 +684,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Создание таблицы в базе данных</t>
+          <t>Создание таблицы в базе данных.</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -702,7 +702,11 @@
           <t>2024-11-19 13:58:50</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr"/>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2024-11-20 12:29:35</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1676,7 +1680,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Вывод текущей латы и времени</t>
+          <t>Вывод текущей даты и времени.</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1684,7 +1688,11 @@
           <t>2024-11-15 13:09:33</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr"/>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>2024-11-20 12:26:54</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1697,14 +1705,40 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Тег h1</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Тег h1 - заголовок первого уровня. Пример написания: &lt;h1&gt;&lt;/h1&gt;</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>2024-11-20 09:36:48</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>2024-11-20 13:47:03</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -3431,7 +3465,7 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Скрипт powershell, который убивает все python запущенные процессы</t>
+          <t>Скрипт powershell, который убивает все python запущенные процессы.</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -3439,7 +3473,11 @@
           <t>2024-11-15 13:18:16</t>
         </is>
       </c>
-      <c r="E80" t="inlineStr"/>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>2024-11-20 16:21:09</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
@@ -3452,7 +3490,7 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Проверка обновлений библиотек</t>
+          <t>Проверка обновлений библиотек!!</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -3460,7 +3498,11 @@
           <t>2024-11-15 13:18:16</t>
         </is>
       </c>
-      <c r="E81" t="inlineStr"/>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>2024-11-20 12:36:21</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3545,7 +3587,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B123"/>
+  <dimension ref="A1:B121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3559,7 +3601,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>option2</t>
+          <t>Samsung</t>
         </is>
       </c>
     </row>
@@ -3569,7 +3611,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>option3</t>
+          <t>AMD</t>
         </is>
       </c>
     </row>
@@ -3579,7 +3621,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Intel</t>
+          <t>ASUS</t>
         </is>
       </c>
     </row>
@@ -3589,7 +3631,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>AMD</t>
+          <t>Acer</t>
         </is>
       </c>
     </row>
@@ -3599,7 +3641,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>HP</t>
+          <t>ASUS</t>
         </is>
       </c>
     </row>
@@ -3609,7 +3651,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>ASUS</t>
         </is>
       </c>
     </row>
@@ -3629,7 +3671,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Acer</t>
+          <t>Samsung</t>
         </is>
       </c>
     </row>
@@ -3639,7 +3681,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Samsung</t>
+          <t>Toyota</t>
         </is>
       </c>
     </row>
@@ -3649,7 +3691,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>ASUS</t>
         </is>
       </c>
     </row>
@@ -3659,7 +3701,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>ASUS</t>
+          <t>HP</t>
         </is>
       </c>
     </row>
@@ -3679,7 +3721,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>HP</t>
+          <t>Intel</t>
         </is>
       </c>
     </row>
@@ -3689,7 +3731,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Intel</t>
+          <t>AMD</t>
         </is>
       </c>
     </row>
@@ -3709,7 +3751,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>AMD</t>
+          <t>Acer</t>
         </is>
       </c>
     </row>
@@ -3719,7 +3761,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>AMD</t>
+          <t>Toyota</t>
         </is>
       </c>
     </row>
@@ -3729,7 +3771,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>HP</t>
         </is>
       </c>
     </row>
@@ -3739,7 +3781,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Samsung</t>
+          <t>Toyota</t>
         </is>
       </c>
     </row>
@@ -3749,7 +3791,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Acer</t>
+          <t>HP</t>
         </is>
       </c>
     </row>
@@ -3769,7 +3811,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>Ford</t>
         </is>
       </c>
     </row>
@@ -3789,7 +3831,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Intel</t>
+          <t>AMD</t>
         </is>
       </c>
     </row>
@@ -3799,7 +3841,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>ASUS</t>
+          <t>Ford</t>
         </is>
       </c>
     </row>
@@ -3819,7 +3861,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>Intel</t>
         </is>
       </c>
     </row>
@@ -3829,7 +3871,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>AMD</t>
+          <t>HP</t>
         </is>
       </c>
     </row>
@@ -3839,7 +3881,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Samsung</t>
+          <t>Acer</t>
         </is>
       </c>
     </row>
@@ -3849,7 +3891,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Acer</t>
+          <t>HP</t>
         </is>
       </c>
     </row>
@@ -3859,7 +3901,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Acer</t>
+          <t>ASUS</t>
         </is>
       </c>
     </row>
@@ -3869,7 +3911,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>HP</t>
+          <t>Acer</t>
         </is>
       </c>
     </row>
@@ -3879,7 +3921,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>Samsung</t>
         </is>
       </c>
     </row>
@@ -3889,7 +3931,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>Toyota</t>
         </is>
       </c>
     </row>
@@ -3899,7 +3941,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Intel</t>
+          <t>Toyota</t>
         </is>
       </c>
     </row>
@@ -3909,7 +3951,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>HP</t>
+          <t>AMD</t>
         </is>
       </c>
     </row>
@@ -3919,7 +3961,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>HP</t>
+          <t>Acer</t>
         </is>
       </c>
     </row>
@@ -3929,7 +3971,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Intel</t>
+          <t>Ford</t>
         </is>
       </c>
     </row>
@@ -3939,7 +3981,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>HP</t>
         </is>
       </c>
     </row>
@@ -3949,7 +3991,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>ASUS</t>
+          <t>Intel</t>
         </is>
       </c>
     </row>
@@ -3959,7 +4001,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>HP</t>
+          <t>Ford</t>
         </is>
       </c>
     </row>
@@ -3969,7 +4011,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>AMD</t>
+          <t>Acer</t>
         </is>
       </c>
     </row>
@@ -3979,7 +4021,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>ASUS</t>
         </is>
       </c>
     </row>
@@ -3999,7 +4041,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Intel</t>
+          <t>HP</t>
         </is>
       </c>
     </row>
@@ -4009,7 +4051,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Samsung</t>
+          <t>Intel</t>
         </is>
       </c>
     </row>
@@ -4019,7 +4061,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>AMD</t>
+          <t>Samsung</t>
         </is>
       </c>
     </row>
@@ -4039,7 +4081,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>AMD</t>
+          <t>Acer</t>
         </is>
       </c>
     </row>
@@ -4049,7 +4091,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>ASUS</t>
+          <t>Ford</t>
         </is>
       </c>
     </row>
@@ -4069,7 +4111,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>ASUS</t>
+          <t>Acer</t>
         </is>
       </c>
     </row>
@@ -4089,7 +4131,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Acer</t>
+          <t>Samsung</t>
         </is>
       </c>
     </row>
@@ -4099,7 +4141,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>AMD</t>
+          <t>Samsung</t>
         </is>
       </c>
     </row>
@@ -4109,7 +4151,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Acer</t>
+          <t>Ford</t>
         </is>
       </c>
     </row>
@@ -4119,7 +4161,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Intel</t>
+          <t>Acer</t>
         </is>
       </c>
     </row>
@@ -4129,7 +4171,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Intel</t>
+          <t>Acer</t>
         </is>
       </c>
     </row>
@@ -4149,7 +4191,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>HP</t>
+          <t>Ford</t>
         </is>
       </c>
     </row>
@@ -4159,7 +4201,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>AMD</t>
+          <t>Toyota</t>
         </is>
       </c>
     </row>
@@ -4169,7 +4211,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>HP</t>
+          <t>Ford</t>
         </is>
       </c>
     </row>
@@ -4179,7 +4221,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Intel</t>
+          <t>Samsung</t>
         </is>
       </c>
     </row>
@@ -4189,7 +4231,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Intel</t>
+          <t>HP</t>
         </is>
       </c>
     </row>
@@ -4199,7 +4241,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>Intel</t>
         </is>
       </c>
     </row>
@@ -4209,7 +4251,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>HP</t>
+          <t>Intel</t>
         </is>
       </c>
     </row>
@@ -4219,7 +4261,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>AMD</t>
+          <t>Toyota</t>
         </is>
       </c>
     </row>
@@ -4229,7 +4271,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Acer</t>
+          <t>AMD</t>
         </is>
       </c>
     </row>
@@ -4249,7 +4291,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>Intel</t>
         </is>
       </c>
     </row>
@@ -4259,7 +4301,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Intel</t>
+          <t>Acer</t>
         </is>
       </c>
     </row>
@@ -4269,7 +4311,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Acer</t>
+          <t>Toyota</t>
         </is>
       </c>
     </row>
@@ -4279,7 +4321,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Samsung</t>
+          <t>Intel</t>
         </is>
       </c>
     </row>
@@ -4289,7 +4331,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>AMD</t>
+          <t>Intel</t>
         </is>
       </c>
     </row>
@@ -4299,7 +4341,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>AMD</t>
+          <t>Ford</t>
         </is>
       </c>
     </row>
@@ -4309,7 +4351,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>ASUS</t>
         </is>
       </c>
     </row>
@@ -4319,7 +4361,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>ASUS</t>
+          <t>Intel</t>
         </is>
       </c>
     </row>
@@ -4329,7 +4371,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>HP</t>
+          <t>Ford</t>
         </is>
       </c>
     </row>
@@ -4339,7 +4381,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>HP</t>
+          <t>ASUS</t>
         </is>
       </c>
     </row>
@@ -4349,7 +4391,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>ASUS</t>
         </is>
       </c>
     </row>
@@ -4359,7 +4401,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>ASUS</t>
+          <t>AMD</t>
         </is>
       </c>
     </row>
@@ -4369,7 +4411,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>Acer</t>
         </is>
       </c>
     </row>
@@ -4379,7 +4421,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>ASUS</t>
+          <t>HP</t>
         </is>
       </c>
     </row>
@@ -4389,7 +4431,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>HP</t>
         </is>
       </c>
     </row>
@@ -4399,7 +4441,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>AMD</t>
         </is>
       </c>
     </row>
@@ -4409,7 +4451,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Intel</t>
+          <t>ASUS</t>
         </is>
       </c>
     </row>
@@ -4419,7 +4461,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Acer</t>
+          <t>AMD</t>
         </is>
       </c>
     </row>
@@ -4439,7 +4481,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>HP</t>
+          <t>Acer</t>
         </is>
       </c>
     </row>
@@ -4449,7 +4491,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>AMD</t>
+          <t>Samsung</t>
         </is>
       </c>
     </row>
@@ -4459,7 +4501,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>HP</t>
+          <t>Toyota</t>
         </is>
       </c>
     </row>
@@ -4469,7 +4511,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>ASUS</t>
+          <t>Ford</t>
         </is>
       </c>
     </row>
@@ -4479,7 +4521,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>AMD</t>
+          <t>Samsung</t>
         </is>
       </c>
     </row>
@@ -4489,7 +4531,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>HP</t>
         </is>
       </c>
     </row>
@@ -4499,7 +4541,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>ASUS</t>
         </is>
       </c>
     </row>
@@ -4509,7 +4551,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Samsung</t>
+          <t>ASUS</t>
         </is>
       </c>
     </row>
@@ -4519,7 +4561,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>AMD</t>
+          <t>Acer</t>
         </is>
       </c>
     </row>
@@ -4529,7 +4571,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>HP</t>
+          <t>Toyota</t>
         </is>
       </c>
     </row>
@@ -4539,7 +4581,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Acer</t>
+          <t>Toyota</t>
         </is>
       </c>
     </row>
@@ -4549,7 +4591,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>HP</t>
+          <t>Intel</t>
         </is>
       </c>
     </row>
@@ -4559,7 +4601,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>ASUS</t>
+          <t>Тестовая запись №1</t>
         </is>
       </c>
     </row>
@@ -4569,7 +4611,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>Тестовая запись №2</t>
         </is>
       </c>
     </row>
@@ -4579,7 +4621,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Тестовая запись №1</t>
+          <t>Тестовая запись №3</t>
         </is>
       </c>
     </row>
@@ -4589,7 +4631,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Тестовая запись №2</t>
+          <t>Тестовая запись №4</t>
         </is>
       </c>
     </row>
@@ -4599,7 +4641,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Тестовая запись №3</t>
+          <t>Тестовая запись №5</t>
         </is>
       </c>
     </row>
@@ -4609,7 +4651,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Тестовая запись №4</t>
+          <t>Тестовая запись №6</t>
         </is>
       </c>
     </row>
@@ -4619,7 +4661,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Тестовая запись №5</t>
+          <t>Тестовая запись №7</t>
         </is>
       </c>
     </row>
@@ -4629,7 +4671,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Тестовая запись №6</t>
+          <t>Тестовая запись №8</t>
         </is>
       </c>
     </row>
@@ -4639,7 +4681,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Тестовая запись №7</t>
+          <t>Тестовая запись №9</t>
         </is>
       </c>
     </row>
@@ -4649,7 +4691,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Тестовая запись №8</t>
+          <t>Тестовая запись №10</t>
         </is>
       </c>
     </row>
@@ -4659,7 +4701,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Тестовая запись №9</t>
+          <t>Тестовая запись №11</t>
         </is>
       </c>
     </row>
@@ -4669,7 +4711,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Тестовая запись №10</t>
+          <t>Тестовая запись №12</t>
         </is>
       </c>
     </row>
@@ -4679,7 +4721,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Тестовая запись №11</t>
+          <t>Тестовая запись №13</t>
         </is>
       </c>
     </row>
@@ -4689,7 +4731,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Тестовая запись №12</t>
+          <t>Тестовая запись №14</t>
         </is>
       </c>
     </row>
@@ -4699,7 +4741,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Тестовая запись №13</t>
+          <t>Тестовая запись №15</t>
         </is>
       </c>
     </row>
@@ -4709,7 +4751,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Тестовая запись №14</t>
+          <t>Тестовая запись №16</t>
         </is>
       </c>
     </row>
@@ -4719,7 +4761,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Тестовая запись №15</t>
+          <t>Тестовая запись №17</t>
         </is>
       </c>
     </row>
@@ -4729,7 +4771,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Тестовая запись №16</t>
+          <t>Тестовая запись №18</t>
         </is>
       </c>
     </row>
@@ -4739,7 +4781,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Тестовая запись №17</t>
+          <t>Тестовая запись №19</t>
         </is>
       </c>
     </row>
@@ -4749,7 +4791,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Тестовая запись №18</t>
+          <t>Тестовая запись №20</t>
         </is>
       </c>
     </row>
@@ -4758,26 +4800,6 @@
         <v>121</v>
       </c>
       <c r="B121" t="inlineStr">
-        <is>
-          <t>Тестовая запись №19</t>
-        </is>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" t="n">
-        <v>122</v>
-      </c>
-      <c r="B122" t="inlineStr">
-        <is>
-          <t>Тестовая запись №20</t>
-        </is>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" t="n">
-        <v>123</v>
-      </c>
-      <c r="B123" t="inlineStr">
         <is>
           <t>option3</t>
         </is>

</xml_diff>

<commit_message>
Hotfix: Mon Nov 25 17:30:37 RTZ 2024
</commit_message>
<xml_diff>
--- a/files/database_tables.xlsx
+++ b/files/database_tables.xlsx
@@ -418,7 +418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -705,6 +705,31 @@
       <c r="E13" t="inlineStr">
         <is>
           <t>2024-11-20 12:29:35</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>1168</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>фвфвыфвфвыфв1</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>фывфывыфвыфвфвф1</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>2024-11-25 13:22:54</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2024-11-25 16:28:26</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Hotfix: Fri Nov 29 14:00:15 RTZ 2024
</commit_message>
<xml_diff>
--- a/files/database_tables.xlsx
+++ b/files/database_tables.xlsx
@@ -3626,7 +3626,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Samsung</t>
+          <t>option1</t>
         </is>
       </c>
     </row>
@@ -3636,7 +3636,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>AMD</t>
+          <t>Тестовая запись №1</t>
         </is>
       </c>
     </row>
@@ -3646,7 +3646,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ASUS</t>
+          <t>Тестовая запись №2</t>
         </is>
       </c>
     </row>
@@ -3656,7 +3656,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Acer</t>
+          <t>Тестовая запись №3</t>
         </is>
       </c>
     </row>
@@ -3666,7 +3666,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ASUS</t>
+          <t>Тестовая запись №4</t>
         </is>
       </c>
     </row>
@@ -3676,7 +3676,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ASUS</t>
+          <t>Тестовая запись №5</t>
         </is>
       </c>
     </row>
@@ -3686,7 +3686,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ASUS</t>
+          <t>Тестовая запись №6</t>
         </is>
       </c>
     </row>
@@ -3696,7 +3696,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Samsung</t>
+          <t>Тестовая запись №7</t>
         </is>
       </c>
     </row>
@@ -3706,7 +3706,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>Тестовая запись №8</t>
         </is>
       </c>
     </row>
@@ -3716,7 +3716,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ASUS</t>
+          <t>Тестовая запись №9</t>
         </is>
       </c>
     </row>
@@ -3726,7 +3726,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>HP</t>
+          <t>Тестовая запись №10</t>
         </is>
       </c>
     </row>
@@ -3736,7 +3736,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>Тестовая запись №11</t>
         </is>
       </c>
     </row>
@@ -3746,7 +3746,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Intel</t>
+          <t>Тестовая запись №12</t>
         </is>
       </c>
     </row>
@@ -3756,7 +3756,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>AMD</t>
+          <t>Тестовая запись №13</t>
         </is>
       </c>
     </row>
@@ -3766,7 +3766,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>ASUS</t>
+          <t>Тестовая запись №14</t>
         </is>
       </c>
     </row>
@@ -3776,7 +3776,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Acer</t>
+          <t>Тестовая запись №15</t>
         </is>
       </c>
     </row>
@@ -3786,7 +3786,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>Тестовая запись №16</t>
         </is>
       </c>
     </row>
@@ -3796,7 +3796,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>HP</t>
+          <t>Тестовая запись №17</t>
         </is>
       </c>
     </row>
@@ -3806,7 +3806,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>Тестовая запись №18</t>
         </is>
       </c>
     </row>
@@ -3816,7 +3816,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>HP</t>
+          <t>Тестовая запись №19</t>
         </is>
       </c>
     </row>
@@ -3826,7 +3826,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Acer</t>
+          <t>Тестовая запись №20</t>
         </is>
       </c>
     </row>
@@ -3836,7 +3836,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>Acer</t>
         </is>
       </c>
     </row>
@@ -3846,7 +3846,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Acer</t>
+          <t>Toyota</t>
         </is>
       </c>
     </row>
@@ -3856,7 +3856,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>AMD</t>
+          <t>HP</t>
         </is>
       </c>
     </row>
@@ -3866,7 +3866,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>HP</t>
         </is>
       </c>
     </row>
@@ -3876,7 +3876,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>HP</t>
+          <t>Toyota</t>
         </is>
       </c>
     </row>
@@ -3886,7 +3886,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Intel</t>
+          <t>ASUS</t>
         </is>
       </c>
     </row>
@@ -3906,7 +3906,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Acer</t>
+          <t>Intel</t>
         </is>
       </c>
     </row>
@@ -3926,7 +3926,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>ASUS</t>
+          <t>Ford</t>
         </is>
       </c>
     </row>
@@ -3936,7 +3936,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Acer</t>
+          <t>Ford</t>
         </is>
       </c>
     </row>
@@ -3946,7 +3946,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Samsung</t>
+          <t>Intel</t>
         </is>
       </c>
     </row>
@@ -3956,7 +3956,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>Samsung</t>
         </is>
       </c>
     </row>
@@ -3966,7 +3966,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>Ford</t>
         </is>
       </c>
     </row>
@@ -3976,7 +3976,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>AMD</t>
+          <t>Toyota</t>
         </is>
       </c>
     </row>
@@ -3986,7 +3986,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Acer</t>
+          <t>AMD</t>
         </is>
       </c>
     </row>
@@ -3996,7 +3996,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>HP</t>
         </is>
       </c>
     </row>
@@ -4006,7 +4006,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>HP</t>
+          <t>Acer</t>
         </is>
       </c>
     </row>
@@ -4016,7 +4016,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Intel</t>
+          <t>Toyota</t>
         </is>
       </c>
     </row>
@@ -4026,7 +4026,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>Toyota</t>
         </is>
       </c>
     </row>
@@ -4036,7 +4036,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Acer</t>
+          <t>Intel</t>
         </is>
       </c>
     </row>
@@ -4046,7 +4046,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>ASUS</t>
+          <t>Ford</t>
         </is>
       </c>
     </row>
@@ -4056,7 +4056,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Samsung</t>
+          <t>Acer</t>
         </is>
       </c>
     </row>
@@ -4066,7 +4066,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>HP</t>
+          <t>Samsung</t>
         </is>
       </c>
     </row>
@@ -4076,7 +4076,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Intel</t>
+          <t>Samsung</t>
         </is>
       </c>
     </row>
@@ -4086,7 +4086,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Samsung</t>
+          <t>Ford</t>
         </is>
       </c>
     </row>
@@ -4096,7 +4096,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Intel</t>
+          <t>ASUS</t>
         </is>
       </c>
     </row>
@@ -4106,7 +4106,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Acer</t>
+          <t>Samsung</t>
         </is>
       </c>
     </row>
@@ -4116,7 +4116,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>Intel</t>
         </is>
       </c>
     </row>
@@ -4136,7 +4136,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Acer</t>
+          <t>Ford</t>
         </is>
       </c>
     </row>
@@ -4146,7 +4146,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>AMD</t>
+          <t>Samsung</t>
         </is>
       </c>
     </row>
@@ -4156,7 +4156,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Samsung</t>
+          <t>HP</t>
         </is>
       </c>
     </row>
@@ -4166,7 +4166,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Samsung</t>
+          <t>HP</t>
         </is>
       </c>
     </row>
@@ -4176,7 +4176,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>ASUS</t>
         </is>
       </c>
     </row>
@@ -4186,7 +4186,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Acer</t>
+          <t>ASUS</t>
         </is>
       </c>
     </row>
@@ -4196,7 +4196,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Acer</t>
+          <t>Ford</t>
         </is>
       </c>
     </row>
@@ -4206,7 +4206,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Intel</t>
+          <t>Acer</t>
         </is>
       </c>
     </row>
@@ -4216,7 +4216,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>Samsung</t>
         </is>
       </c>
     </row>
@@ -4226,7 +4226,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>HP</t>
         </is>
       </c>
     </row>
@@ -4236,7 +4236,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>Toyota</t>
         </is>
       </c>
     </row>
@@ -4246,7 +4246,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Samsung</t>
+          <t>AMD</t>
         </is>
       </c>
     </row>
@@ -4256,7 +4256,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>HP</t>
+          <t>Acer</t>
         </is>
       </c>
     </row>
@@ -4266,7 +4266,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Intel</t>
+          <t>ASUS</t>
         </is>
       </c>
     </row>
@@ -4276,7 +4276,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Intel</t>
+          <t>Acer</t>
         </is>
       </c>
     </row>
@@ -4286,7 +4286,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>ASUS</t>
         </is>
       </c>
     </row>
@@ -4296,7 +4296,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>AMD</t>
+          <t>ASUS</t>
         </is>
       </c>
     </row>
@@ -4306,7 +4306,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>AMD</t>
+          <t>Acer</t>
         </is>
       </c>
     </row>
@@ -4316,7 +4316,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Intel</t>
+          <t>HP</t>
         </is>
       </c>
     </row>
@@ -4326,7 +4326,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Acer</t>
+          <t>Samsung</t>
         </is>
       </c>
     </row>
@@ -4336,7 +4336,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>AMD</t>
         </is>
       </c>
     </row>
@@ -4346,7 +4346,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Intel</t>
+          <t>Samsung</t>
         </is>
       </c>
     </row>
@@ -4356,7 +4356,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Intel</t>
+          <t>Toyota</t>
         </is>
       </c>
     </row>
@@ -4366,7 +4366,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>HP</t>
         </is>
       </c>
     </row>
@@ -4376,7 +4376,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>ASUS</t>
+          <t>Samsung</t>
         </is>
       </c>
     </row>
@@ -4386,7 +4386,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Intel</t>
+          <t>Ford</t>
         </is>
       </c>
     </row>
@@ -4396,7 +4396,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>HP</t>
         </is>
       </c>
     </row>
@@ -4406,7 +4406,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>ASUS</t>
+          <t>Ford</t>
         </is>
       </c>
     </row>
@@ -4416,7 +4416,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>ASUS</t>
+          <t>Samsung</t>
         </is>
       </c>
     </row>
@@ -4436,7 +4436,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Acer</t>
+          <t>HP</t>
         </is>
       </c>
     </row>
@@ -4446,7 +4446,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>HP</t>
+          <t>AMD</t>
         </is>
       </c>
     </row>
@@ -4456,7 +4456,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>HP</t>
+          <t>Samsung</t>
         </is>
       </c>
     </row>
@@ -4476,7 +4476,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>ASUS</t>
+          <t>AMD</t>
         </is>
       </c>
     </row>
@@ -4486,7 +4486,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>AMD</t>
+          <t>Samsung</t>
         </is>
       </c>
     </row>
@@ -4496,7 +4496,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>AMD</t>
+          <t>Acer</t>
         </is>
       </c>
     </row>
@@ -4516,7 +4516,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Samsung</t>
+          <t>Intel</t>
         </is>
       </c>
     </row>
@@ -4526,7 +4526,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>Samsung</t>
         </is>
       </c>
     </row>
@@ -4536,7 +4536,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>Acer</t>
         </is>
       </c>
     </row>
@@ -4546,7 +4546,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Samsung</t>
+          <t>HP</t>
         </is>
       </c>
     </row>
@@ -4576,7 +4576,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>ASUS</t>
+          <t>Toyota</t>
         </is>
       </c>
     </row>
@@ -4586,7 +4586,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Acer</t>
+          <t>Samsung</t>
         </is>
       </c>
     </row>
@@ -4596,7 +4596,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>Samsung</t>
         </is>
       </c>
     </row>
@@ -4606,7 +4606,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>Samsung</t>
         </is>
       </c>
     </row>
@@ -4616,7 +4616,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Intel</t>
+          <t>Samsung</t>
         </is>
       </c>
     </row>
@@ -4626,7 +4626,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Тестовая запись №1</t>
+          <t>Acer</t>
         </is>
       </c>
     </row>
@@ -4636,7 +4636,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Тестовая запись №2</t>
+          <t>Intel</t>
         </is>
       </c>
     </row>
@@ -4646,7 +4646,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Тестовая запись №3</t>
+          <t>Intel</t>
         </is>
       </c>
     </row>
@@ -4656,7 +4656,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Тестовая запись №4</t>
+          <t>Acer</t>
         </is>
       </c>
     </row>
@@ -4666,7 +4666,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Тестовая запись №5</t>
+          <t>Samsung</t>
         </is>
       </c>
     </row>
@@ -4676,7 +4676,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Тестовая запись №6</t>
+          <t>Ford</t>
         </is>
       </c>
     </row>
@@ -4686,7 +4686,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Тестовая запись №7</t>
+          <t>Acer</t>
         </is>
       </c>
     </row>
@@ -4696,7 +4696,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Тестовая запись №8</t>
+          <t>Samsung</t>
         </is>
       </c>
     </row>
@@ -4706,7 +4706,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Тестовая запись №9</t>
+          <t>AMD</t>
         </is>
       </c>
     </row>
@@ -4716,7 +4716,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Тестовая запись №10</t>
+          <t>Toyota</t>
         </is>
       </c>
     </row>
@@ -4726,7 +4726,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Тестовая запись №11</t>
+          <t>HP</t>
         </is>
       </c>
     </row>
@@ -4736,7 +4736,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Тестовая запись №12</t>
+          <t>Ford</t>
         </is>
       </c>
     </row>
@@ -4746,7 +4746,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Тестовая запись №13</t>
+          <t>Samsung</t>
         </is>
       </c>
     </row>
@@ -4756,7 +4756,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Тестовая запись №14</t>
+          <t>Acer</t>
         </is>
       </c>
     </row>
@@ -4766,7 +4766,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Тестовая запись №15</t>
+          <t>Ford</t>
         </is>
       </c>
     </row>
@@ -4776,7 +4776,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Тестовая запись №16</t>
+          <t>Toyota</t>
         </is>
       </c>
     </row>
@@ -4786,7 +4786,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Тестовая запись №17</t>
+          <t>Toyota</t>
         </is>
       </c>
     </row>
@@ -4796,7 +4796,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Тестовая запись №18</t>
+          <t>Acer</t>
         </is>
       </c>
     </row>
@@ -4806,7 +4806,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Тестовая запись №19</t>
+          <t>ASUS</t>
         </is>
       </c>
     </row>
@@ -4816,7 +4816,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Тестовая запись №20</t>
+          <t>Samsung</t>
         </is>
       </c>
     </row>
@@ -4826,7 +4826,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>option3</t>
+          <t>Acer</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Commit: 20 янв 2025 г. 15:54:43
</commit_message>
<xml_diff>
--- a/files/database_tables.xlsx
+++ b/files/database_tables.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F125"/>
+  <dimension ref="A1:F126"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3437,6 +3437,30 @@
       </c>
       <c r="F125" t="inlineStr"/>
     </row>
+    <row r="126">
+      <c r="A126" t="n">
+        <v>146</v>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>cd /g</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>Переход на другой диск, в данном случае диск g:</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>cli</t>
+        </is>
+      </c>
+      <c r="E126" s="1" t="n">
+        <v>45677.64894675926</v>
+      </c>
+      <c r="F126" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Commit: 23 янв 2025 г. 12:03:10
</commit_message>
<xml_diff>
--- a/files/database_tables.xlsx
+++ b/files/database_tables.xlsx
@@ -20,13 +20,16 @@
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
     <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +40,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,12 +48,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -417,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F126"/>
+  <dimension ref="A1:F127"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,41 +438,49 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>CTRL + U</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Удаление последней набранной строки</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>cli</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="n">
-        <v>45642.50591435185</v>
-      </c>
-      <c r="F1" t="inlineStr"/>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>category</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>date_add</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>date_edit</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>CTRL + R</t>
+          <t>CTRL + U</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Поиск текста в истории</t>
+          <t>Удаление последней набранной строки</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -468,23 +488,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E2" s="1" t="n">
+      <c r="E2" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>cp bash_and_git.txt ~/draft-project</t>
+          <t>CTRL + R</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Копирование файлов</t>
+          <t>Поиск текста в истории</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -492,23 +512,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="E3" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>clear</t>
+          <t>cp bash_and_git.txt ~/draft-project</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Очистка экрана</t>
+          <t>Копирование файлов</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -516,23 +536,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E4" s="1" t="n">
+      <c r="E4" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>kill 666</t>
+          <t>clear</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Завершает процесс</t>
+          <t>Очистка экрана</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -540,23 +560,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E5" s="1" t="n">
+      <c r="E5" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>history</t>
+          <t>kill 666</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>История команд</t>
+          <t>Завершает процесс</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -564,23 +584,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E6" s="1" t="n">
+      <c r="E6" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ps</t>
+          <t>history</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Выводит список процессов</t>
+          <t>История команд</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -588,23 +608,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E7" s="1" t="n">
+      <c r="E7" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>pwd</t>
+          <t>ps</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Показывает текущий путь к папке</t>
+          <t>Выводит список процессов</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -612,23 +632,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E8" s="1" t="n">
+      <c r="E8" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>cd ..</t>
+          <t>pwd</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Возврат в вышестоящую директорию</t>
+          <t>Показывает текущий путь к папке</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -636,23 +656,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E9" s="1" t="n">
+      <c r="E9" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>cd ../..</t>
+          <t>cd ..</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Возврат на две папки выше</t>
+          <t>Возврат в вышестоящую директорию</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -660,23 +680,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E10" s="1" t="n">
+      <c r="E10" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>cd ~</t>
+          <t>cd ../..</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Переход в корневую папку</t>
+          <t>Возврат на две папки выше</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -684,23 +704,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E11" s="1" t="n">
+      <c r="E11" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>ls</t>
+          <t>cd ~</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Вывод содержимого каталога(файлов и папок)</t>
+          <t>Переход в корневую папку</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -708,23 +728,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E12" s="1" t="n">
+      <c r="E12" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>cd -</t>
+          <t>ls</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Вернуться назад</t>
+          <t>Вывод содержимого каталога(файлов и папок)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -732,23 +752,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E13" s="1" t="n">
+      <c r="E13" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>cd Users/</t>
+          <t>cd -</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Переход  в оперделенную папку</t>
+          <t>Вернуться назад</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -756,23 +776,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E14" s="1" t="n">
+      <c r="E14" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>ls -f</t>
+          <t>cd Users/</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Показать файлы в данной папке, включая и скрытые</t>
+          <t>Переход  в определенную папку, в этом случае в папку Users</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -780,23 +800,27 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E15" s="1" t="n">
-        <v>45642.50591435185</v>
-      </c>
-      <c r="F15" t="inlineStr"/>
+      <c r="E15" s="2" t="n">
+        <v>45642.50591435185</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2025-01-21 14:53:07</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>ls -d */</t>
+          <t>ls -f</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Вывод папок раздела</t>
+          <t>Показать файлы в данной папке, включая скрытые</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -804,23 +828,27 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E16" s="1" t="n">
-        <v>45642.50591435185</v>
-      </c>
-      <c r="F16" t="inlineStr"/>
+      <c r="E16" s="2" t="n">
+        <v>45642.50591435185</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2025-01-21 15:10:02</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>mkdir folder</t>
+          <t>ls -d */</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Создание папки или папок(несколько папок через пробел нужно указать)</t>
+          <t>Вывод папок раздела</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -828,23 +856,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E17" s="1" t="n">
+      <c r="E17" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>mv intro manual/chap1</t>
+          <t>mkdir folder</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Файл intro перенесется в папку manual под именем chap1</t>
+          <t>Создание папки или папок(несколько папок через пробел нужно указать)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -852,23 +880,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E18" s="1" t="n">
+      <c r="E18" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>mv chap3 manual</t>
+          <t>mv intro manual/chap1</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Файл chap3 перенесется в папку manual</t>
+          <t>Файл intro перенесется в папку manual под именем chap1</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -876,23 +904,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E19" s="1" t="n">
+      <c r="E19" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>mv appendix apndx.a</t>
+          <t>mv chap3 manual</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Файл appendix переименуется в apndx.a</t>
+          <t>Файл chap3 перенесется в папку manual</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -900,23 +928,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E20" s="1" t="n">
+      <c r="E20" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>cat id_ed25519.pub</t>
+          <t>mv appendix apndx.a</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Чтение указанного файла</t>
+          <t>Файл appendix переименуется в apndx.a</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -924,23 +952,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E21" s="1" t="n">
+      <c r="E21" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>rm myfile</t>
+          <t>cat id_ed25519.pub</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Удаление файла</t>
+          <t>Чтение указанного файла</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -948,23 +976,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E22" s="1" t="n">
+      <c r="E22" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>rm -R GitHub/</t>
+          <t>rm myfile</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Удаление папки с содержанием</t>
+          <t>Удаление файла</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -972,23 +1000,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E23" s="1" t="n">
+      <c r="E23" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>rm -f -R GitHub/</t>
+          <t>rm -R GitHub/</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Удаление папки с содержанием принудительно</t>
+          <t>Удаление папки с содержанием</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -996,23 +1024,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E24" s="1" t="n">
+      <c r="E24" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>exit</t>
+          <t>rm -f -R GitHub/</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Выход из командной строки</t>
+          <t>Удаление папки с содержанием принудительно</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1020,23 +1048,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E25" s="1" t="n">
+      <c r="E25" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>nslookup test.ru</t>
+          <t>exit</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Запрос DNS определенного адреса</t>
+          <t>Выход из командной строки</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1044,23 +1072,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E26" s="1" t="n">
+      <c r="E26" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>flask_project_lite_version/venv/scripts/python.exe flask_project_lite_version/app.py &amp;</t>
+          <t>nslookup test.ru</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Запуск процесса в фоновом режиме</t>
+          <t>Запрос DNS определенного адреса</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1068,23 +1096,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E27" s="1" t="n">
+      <c r="E27" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>ssh-keygen</t>
+          <t>flask_project_lite_version/venv/scripts/python.exe flask_project_lite_version/app.py &amp;</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Генерация ssh-ключа</t>
+          <t>Запуск процесса в фоновом режиме</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1092,23 +1120,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E28" s="1" t="n">
+      <c r="E28" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>python -m venv venv</t>
+          <t>ssh-keygen</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Создание виртуального окружения Python</t>
+          <t>Генерация ssh-ключа</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1116,23 +1144,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E29" s="1" t="n">
+      <c r="E29" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>touch bash.sh</t>
+          <t>python -m venv venv</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Создание файла скрипта bash.sh</t>
+          <t>Создание виртуального окружения Python</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1140,23 +1168,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E30" s="1" t="n">
+      <c r="E30" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>nano bash.sh</t>
+          <t>touch bash.sh</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Открытие файла встроенным bash редактором</t>
+          <t>Создание файла скрипта bash.sh</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1164,23 +1192,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E31" s="1" t="n">
+      <c r="E31" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>./bash.sh</t>
+          <t>nano bash.sh</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Запуск скрипта bash</t>
+          <t>Открытие файла встроенным bash редактором</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1188,23 +1216,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E32" s="1" t="n">
+      <c r="E32" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>cmod +x bash.sh</t>
+          <t>./bash.sh</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Настройка прав на файл скрипта</t>
+          <t>Запуск скрипта bash</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1212,23 +1240,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E33" s="1" t="n">
+      <c r="E33" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>ls -l</t>
+          <t>cmod +x bash.sh</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Выводит списокм папки и файлы текущего раздела с датой изменения, размером и правами доступа</t>
+          <t>Настройка прав на файл скрипта</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1236,23 +1264,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E34" s="1" t="n">
+      <c r="E34" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>rm *</t>
+          <t>ls -l</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Удаляет все файлы в текущей директории</t>
+          <t>Выводит на экран списком папки и файлы текущего раздела с датой изменения, размером и правами доступа</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1260,23 +1288,27 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E35" s="1" t="n">
-        <v>45642.50591435185</v>
-      </c>
-      <c r="F35" t="inlineStr"/>
+      <c r="E35" s="2" t="n">
+        <v>45642.50591435185</v>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>2025-01-21 15:10:32</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>history -c</t>
+          <t>rm *</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Удаляет все команды из истории</t>
+          <t>Удаляет все файлы в текущей директории</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1284,23 +1316,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E36" s="1" t="n">
+      <c r="E36" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>history -c</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Вывод текущей даты и времени</t>
+          <t>Удаляет все команды из истории</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1308,23 +1340,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E37" s="1" t="n">
+      <c r="E37" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>mkdir test1 test2</t>
+          <t>date</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Создаем две папки в текущем каталоге</t>
+          <t>Вывод текущей даты и времени</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1332,23 +1364,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E38" s="1" t="n">
+      <c r="E38" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>rm -R *</t>
+          <t>mkdir test1 test2</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Удаление всех папок текущей директории</t>
+          <t>Создаем две папки в текущем каталоге</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1356,23 +1388,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E39" s="1" t="n">
+      <c r="E39" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>~/AppData/Local/Programs/Python/Python312/python.exe venv/Scripts/pip.exe install flask-paginate</t>
+          <t>rm -R *</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Установки нужной библиотеки</t>
+          <t>Удаление всех папок текущей директории</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1380,23 +1412,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E40" s="1" t="n">
+      <c r="E40" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>cd /p/s.savin/flask-project-full/</t>
+          <t>~/AppData/Local/Programs/Python/Python312/python.exe venv/Scripts/pip.exe install flask-paginate</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Переход из текущего раздела в другой раздел с определенной папкой</t>
+          <t>Установки нужной библиотеки</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1404,23 +1436,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E41" s="1" t="n">
+      <c r="E41" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>ls *.sh</t>
+          <t>cd /p/s.savin/flask-project-full/</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Выводит на экран все файлы с указанным расширением</t>
+          <t>Переход из текущего раздела в другой раздел с определенной папкой</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1428,23 +1460,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E42" s="1" t="n">
+      <c r="E42" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>cd</t>
+          <t>ls *.sh</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Вернуться в корневую папку</t>
+          <t>Выводит на экран все файлы с указанным расширением</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1452,23 +1484,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E43" s="1" t="n">
+      <c r="E43" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>cp -r ~/dbeaver-ce-24.0.4-win32.win32.x86_64/dbeaver/bases* /p/home/</t>
+          <t>cd</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Копирование всех файлов в другую папку</t>
+          <t>Вернуться в корневую папку</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1476,23 +1508,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E44" s="1" t="n">
+      <c r="E44" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>ps | grep python</t>
+          <t>cp -r ~/dbeaver-ce-24.0.4-win32.win32.x86_64/dbeaver/bases* /p/home/</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Поиск процесса по имени</t>
+          <t>Копирование всех файлов в другую папку</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1500,23 +1532,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E45" s="1" t="n">
+      <c r="E45" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>kill -9 $(ps | grep python)</t>
+          <t>ps | grep python</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Завершить работы всех приложений python</t>
+          <t>Поиск процесса по имени</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1524,23 +1556,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E46" s="1" t="n">
+      <c r="E46" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Get-Process python</t>
+          <t>kill -9 $(ps | grep python)</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Вывод всех процессов Windows по имени</t>
+          <t>Завершить работы всех приложений python</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1548,23 +1580,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E47" s="1" t="n">
+      <c r="E47" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t xml:space="preserve">Stop-Process -Name "python" </t>
+          <t>Get-Process python</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Остановка процессов по имени</t>
+          <t>Вывод всех процессов Windows по имени</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1572,23 +1604,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E48" s="1" t="n">
+      <c r="E48" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Remove-Item -LiteralPath '.\Polarity Portable\' -Recurse</t>
+          <t xml:space="preserve">Stop-Process -Name "python" </t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Удаление папки с файлами в PowerShell</t>
+          <t>Остановка процессов по имени</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -1596,23 +1628,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E49" s="1" t="n">
+      <c r="E49" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>python -m  pip freeze &gt; requirements.txt</t>
+          <t>Remove-Item -LiteralPath '.\Polarity Portable\' -Recurse</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Создание файла с пакетами</t>
+          <t>Удаление папки с файлами в PowerShell</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -1620,16 +1652,40 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E50" s="1" t="n">
+      <c r="E50" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="n">
+        <v>51</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>python -m  pip freeze &gt; requirements.txt</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Создание файла с пакетами</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>cli</t>
+        </is>
+      </c>
+      <c r="E51" s="2" t="n">
+        <v>45642.50591435185</v>
+      </c>
+      <c r="F51" t="inlineStr"/>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
         <v>52</v>
       </c>
-      <c r="B51" t="inlineStr">
+      <c r="B52" t="inlineStr">
         <is>
           <t>Вариант использования с виртуальным окружением:
 ~/AppData/Local/Programs/Python/Python312/python.exe venv/Scripts/pip.exe install -r requirements.txt
@@ -1637,57 +1693,33 @@
 pip install -r requirements.txt</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
+      <c r="C52" t="inlineStr">
         <is>
           <t>Устанавливает из файла все пакеты</t>
         </is>
       </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>cli</t>
-        </is>
-      </c>
-      <c r="E51" s="1" t="n">
-        <v>45642.50591435185</v>
-      </c>
-      <c r="F51" t="inlineStr"/>
-    </row>
-    <row r="52">
-      <c r="A52" t="n">
-        <v>53</v>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>mv ReferenceCard.pdf ../</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>Перемещение файла из текущей папки в вышестоящий раздел</t>
-        </is>
-      </c>
       <c r="D52" t="inlineStr">
         <is>
           <t>cli</t>
         </is>
       </c>
-      <c r="E52" s="1" t="n">
+      <c r="E52" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>mv *.sh virtual_machine_scripts/</t>
+          <t>mv ReferenceCard.pdf ../</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Перемещение нескольких файлов в другую папку с определенным расширением</t>
+          <t>Перемещение файла из текущей папки в вышестоящий раздел</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -1695,23 +1727,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E53" s="1" t="n">
+      <c r="E53" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>p:/virtual_machine_scripts/start_apps.sh</t>
+          <t>mv *.sh virtual_machine_scripts/</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Запуск bash скрипта из любой директории</t>
+          <t>Перемещение нескольких файлов в другую папку с определенным расширением</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -1719,23 +1751,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E54" s="1" t="n">
+      <c r="E54" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>git config --global user.email "s.savin1@gitlab.plagate.ru"</t>
+          <t>p:/virtual_machine_scripts/start_apps.sh</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Назначение git глобальной почты</t>
+          <t>Запуск bash скрипта из любой директории</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -1743,23 +1775,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E55" s="1" t="n">
+      <c r="E55" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>git config --global user.name "s.savin1"</t>
+          <t>git config --global user.email "s.savin1@gitlab.plagate.ru"</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Назначение git глобального имени</t>
+          <t>Назначение git глобальной почты</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -1767,23 +1799,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E56" s="1" t="n">
+      <c r="E56" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>git clone адрес ссылки</t>
+          <t>git config --global user.name "s.savin1"</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Клонирование удаленного репозитория</t>
+          <t>Назначение git глобального имени</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -1791,23 +1823,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E57" s="1" t="n">
+      <c r="E57" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>git status</t>
+          <t>git clone адрес ссылки</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Статус изменений</t>
+          <t>Клонирование удаленного репозитория</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -1815,23 +1847,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E58" s="1" t="n">
+      <c r="E58" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>git config --list</t>
+          <t>git status</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Вывод конфигурации git</t>
+          <t>Статус изменений</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -1839,23 +1871,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E59" s="1" t="n">
+      <c r="E59" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>git add .</t>
+          <t>git config --list</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Подготовка файлов для коммита</t>
+          <t>Вывод конфигурации git</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -1863,23 +1895,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E60" s="1" t="n">
+      <c r="E60" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>git commit -m "test"</t>
+          <t>git add .</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Подготовка коммита</t>
+          <t>Подготовка файлов для коммита</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -1887,23 +1919,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E61" s="1" t="n">
+      <c r="E61" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>git push</t>
+          <t>git commit -m "test"</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Отправка изменений на репозиторий</t>
+          <t>Подготовка коммита</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -1911,23 +1943,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E62" s="1" t="n">
+      <c r="E62" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>git init</t>
+          <t>git push</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Инициализация git в папке</t>
+          <t>Отправка изменений на репозиторий</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -1935,23 +1967,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E63" s="1" t="n">
+      <c r="E63" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>git pull</t>
+          <t>git init</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Скачивание изменения из репозитория на локальную машину</t>
+          <t>Инициализация git в папке</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -1959,23 +1991,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E64" s="1" t="n">
+      <c r="E64" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>~/AppData/Local/Programs/Python/Python39/python.exe -m pip install --upgrade pip</t>
+          <t>git pull</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Обновление pip</t>
+          <t>Скачивание изменения из репозитория на локальную машину</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -1983,23 +2015,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E65" s="1" t="n">
+      <c r="E65" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>~/AppData/Local/Programs/Python/Python39/python.exe venv/Scripts/pip.exe install pandas</t>
+          <t>~/AppData/Local/Programs/Python/Python39/python.exe -m pip install --upgrade pip</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Установка библиотеки Pandas</t>
+          <t>Обновление pip</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -2007,23 +2039,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E66" s="1" t="n">
+      <c r="E66" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>rename "test.xlsx" "test1.xlsx"</t>
+          <t>~/AppData/Local/Programs/Python/Python39/python.exe venv/Scripts/pip.exe install pandas</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Переименование файла в CMD</t>
+          <t>Установка библиотеки Pandas</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -2031,23 +2063,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E67" s="1" t="n">
+      <c r="E67" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>mount</t>
+          <t>rename "test.xlsx" "test1.xlsx"</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Вывод всех подключенных дисков</t>
+          <t>Переименование файла в CMD</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -2055,23 +2087,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E68" s="1" t="n">
+      <c r="E68" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>tar -cf flask-project.tar * &amp;&amp; mv flask-project.tar /o</t>
+          <t>mount</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Скрипт архивации файлов и перенос архива на другой диск</t>
+          <t>Вывод всех подключенных дисков</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -2079,23 +2111,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E69" s="1" t="n">
+      <c r="E69" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>tar -cf flask-project.tar *</t>
+          <t>tar -cf flask-project.tar * &amp;&amp; mv flask-project.tar /o</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Создание архива всех файлов в папке</t>
+          <t>Скрипт архивации файлов и перенос архива на другой диск</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -2103,23 +2135,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E70" s="1" t="n">
+      <c r="E70" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>mv flask-project.tar /o</t>
+          <t>tar -cf flask-project.tar *</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Перенос файла на другой диск</t>
+          <t>Создание архива всех файлов в папке</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -2127,23 +2159,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E71" s="1" t="n">
+      <c r="E71" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>~/AppData/Local/Programs/Python/Python313/python.exe -m webbrowser http://127.0.0.1:82</t>
+          <t>mv flask-project.tar /o</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Запуск приложения в браузере</t>
+          <t>Перенос файла на другой диск</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -2151,23 +2183,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E72" s="1" t="n">
+      <c r="E72" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Set-ExecutionPolicy RemoteSigned</t>
+          <t>~/AppData/Local/Programs/Python/Python313/python.exe -m webbrowser http://127.0.0.1:82</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Разрешение запуска сценариев powershell</t>
+          <t>Запуск приложения в браузере</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -2175,145 +2207,145 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E73" s="1" t="n">
+      <c r="E73" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="n">
+        <v>78</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Set-ExecutionPolicy RemoteSigned</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Разрешение запуска сценариев powershell</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>cli</t>
+        </is>
+      </c>
+      <c r="E74" s="2" t="n">
+        <v>45642.50591435185</v>
+      </c>
+      <c r="F74" t="inlineStr"/>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
         <v>79</v>
       </c>
-      <c r="B74" t="inlineStr">
+      <c r="B75" t="inlineStr">
         <is>
           <t>where powershell</t>
         </is>
       </c>
-      <c r="C74" t="inlineStr">
+      <c r="C75" t="inlineStr">
         <is>
           <t>Как найти исполняемый файл powershell в системе?
 Ввести в cmd команду!</t>
         </is>
       </c>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t>cli</t>
-        </is>
-      </c>
-      <c r="E74" s="1" t="n">
-        <v>45642.50591435185</v>
-      </c>
-      <c r="F74" t="inlineStr"/>
-    </row>
-    <row r="75">
-      <c r="A75" t="n">
-        <v>80</v>
-      </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>python -m pip uninstall -r requirements.txt -y</t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Принудительное деинсталляция пакетов из файла requirements.txt </t>
-        </is>
-      </c>
       <c r="D75" t="inlineStr">
         <is>
           <t>cli</t>
         </is>
       </c>
-      <c r="E75" s="1" t="n">
+      <c r="E75" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="n">
+        <v>80</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>python -m pip uninstall -r requirements.txt -y</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Принудительное деинсталляция пакетов из файла requirements.txt </t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>cli</t>
+        </is>
+      </c>
+      <c r="E76" s="2" t="n">
+        <v>45642.50591435185</v>
+      </c>
+      <c r="F76" t="inlineStr"/>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
         <v>81</v>
       </c>
-      <c r="B76" t="inlineStr">
+      <c r="B77" t="inlineStr">
         <is>
           <t>#!/c/Windows/System32/WindowsPowerShell/v1.0/powershell.exe
 Stop-Process -Name "python"</t>
         </is>
       </c>
-      <c r="C76" t="inlineStr">
+      <c r="C77" t="inlineStr">
         <is>
           <t>Скрипт powershell, который убивает все python запущенные процессы.</t>
         </is>
       </c>
-      <c r="D76" t="inlineStr">
-        <is>
-          <t>cli</t>
-        </is>
-      </c>
-      <c r="E76" s="1" t="n">
-        <v>45642.50591435185</v>
-      </c>
-      <c r="F76" t="inlineStr"/>
-    </row>
-    <row r="77">
-      <c r="A77" t="n">
-        <v>82</v>
-      </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>pip install --upgrade -r requirements.txt</t>
-        </is>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>Проверка обновлений библиотек!!</t>
-        </is>
-      </c>
       <c r="D77" t="inlineStr">
         <is>
           <t>cli</t>
         </is>
       </c>
-      <c r="E77" s="1" t="n">
+      <c r="E77" s="2" t="n">
         <v>45642.50591435185</v>
       </c>
       <c r="F77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>print(type(count_person))</t>
+          <t>pip install --upgrade -r requirements.txt</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Выводит тип данных</t>
+          <t>Проверка обновлений библиотек!!</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>python</t>
-        </is>
-      </c>
-      <c r="E78" s="1" t="n">
-        <v>45643.50651620371</v>
+          <t>cli</t>
+        </is>
+      </c>
+      <c r="E78" s="2" t="n">
+        <v>45642.50591435185</v>
       </c>
       <c r="F78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>df.to_csv("saved_ratings.csv", index=False))</t>
+          <t>print(type(count_person))</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Экспорт в формат CSV</t>
+          <t>Выводит тип данных</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -2321,23 +2353,23 @@
           <t>python</t>
         </is>
       </c>
-      <c r="E79" s="1" t="n">
+      <c r="E79" s="2" t="n">
         <v>45643.50651620371</v>
       </c>
       <c r="F79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>data_copy = data.copy(deep=True)</t>
+          <t>df.to_csv("saved_ratings.csv", index=False))</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Копирование датафрейма</t>
+          <t>Экспорт в формат CSV</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -2345,23 +2377,23 @@
           <t>python</t>
         </is>
       </c>
-      <c r="E80" s="1" t="n">
+      <c r="E80" s="2" t="n">
         <v>45643.50651620371</v>
       </c>
       <c r="F80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>len(data)</t>
+          <t>data_copy = data.copy(deep=True)</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Подсчёт количества строк в датафрейме</t>
+          <t>Копирование датафрейма</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -2369,23 +2401,23 @@
           <t>python</t>
         </is>
       </c>
-      <c r="E81" s="1" t="n">
+      <c r="E81" s="2" t="n">
         <v>45643.50651620371</v>
       </c>
       <c r="F81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>len(data["user_id"].unique())</t>
+          <t>len(data)</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Подсчёт количества уникальных значений в столбце</t>
+          <t>Подсчёт количества строк в датафрейме</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -2393,23 +2425,23 @@
           <t>python</t>
         </is>
       </c>
-      <c r="E82" s="1" t="n">
+      <c r="E82" s="2" t="n">
         <v>45643.50651620371</v>
       </c>
       <c r="F82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>data.describe()</t>
+          <t>len(data["user_id"].unique())</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Вывод статистических сведений о датафрейме</t>
+          <t>Подсчёт количества уникальных значений в столбце</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -2417,23 +2449,23 @@
           <t>python</t>
         </is>
       </c>
-      <c r="E83" s="1" t="n">
+      <c r="E83" s="2" t="n">
         <v>45643.50651620371</v>
       </c>
       <c r="F83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>data.type.value_counts()</t>
+          <t>data.describe()</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Для того чтобы подсчитать количество значений в конкретном столбце, можно воспользоваться следующей конструкцие</t>
+          <t>Вывод статистических сведений о датафрейме</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -2441,23 +2473,23 @@
           <t>python</t>
         </is>
       </c>
-      <c r="E84" s="1" t="n">
+      <c r="E84" s="2" t="n">
         <v>45643.50651620371</v>
       </c>
       <c r="F84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>data.columns.tolist()</t>
+          <t>data.type.value_counts()</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Получение списка значений столбцов</t>
+          <t>Для того чтобы подсчитать количество значений в конкретном столбце, можно воспользоваться следующей конструкцие</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -2465,23 +2497,23 @@
           <t>python</t>
         </is>
       </c>
-      <c r="E85" s="1" t="n">
+      <c r="E85" s="2" t="n">
         <v>45643.50651620371</v>
       </c>
       <c r="F85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>data["genre"].tolist()</t>
+          <t>data.columns.tolist()</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Создание списка или объекта Series на основе значений столбца</t>
+          <t>Получение списка значений столбцов</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -2489,23 +2521,23 @@
           <t>python</t>
         </is>
       </c>
-      <c r="E86" s="1" t="n">
+      <c r="E86" s="2" t="n">
         <v>45643.50651620371</v>
       </c>
       <c r="F86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>data["train set"] = True</t>
+          <t>data["genre"].tolist()</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Присоединение к датафрейму нового столбца с заданным значением</t>
+          <t>Создание списка или объекта Series на основе значений столбца</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
@@ -2513,23 +2545,23 @@
           <t>python</t>
         </is>
       </c>
-      <c r="E87" s="1" t="n">
+      <c r="E87" s="2" t="n">
         <v>45643.50651620371</v>
       </c>
       <c r="F87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>data[["name","episodes"]]</t>
+          <t>data["train set"] = True</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Создание нового датафрейма из подмножества столбцов</t>
+          <t>Присоединение к датафрейму нового столбца с заданным значением</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -2537,23 +2569,23 @@
           <t>python</t>
         </is>
       </c>
-      <c r="E88" s="1" t="n">
+      <c r="E88" s="2" t="n">
         <v>45643.50651620371</v>
       </c>
       <c r="F88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>data.drop(["density"], axis="columns")</t>
+          <t>data[["name","episodes"]]</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Удаление столбца</t>
+          <t>Создание нового датафрейма из подмножества столбцов</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -2561,23 +2593,23 @@
           <t>python</t>
         </is>
       </c>
-      <c r="E89" s="1" t="n">
+      <c r="E89" s="2" t="n">
         <v>45643.50651620371</v>
       </c>
       <c r="F89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>data_modified.iloc[0:3]</t>
+          <t>data.drop(["density"], axis="columns")</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Получение строк по числовым индексам</t>
+          <t>Удаление столбца</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -2585,23 +2617,23 @@
           <t>python</t>
         </is>
       </c>
-      <c r="E90" s="1" t="n">
+      <c r="E90" s="2" t="n">
         <v>45643.50651620371</v>
       </c>
       <c r="F90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>data[data["type"].isin(["TV", "Movie"])]</t>
+          <t>data_modified.iloc[0:3]</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Для получения строк датафрейма в ситуации, когда имеется список значений столбцов, можно воспользоваться следующей командой</t>
+          <t>Получение строк по числовым индексам</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
@@ -2609,23 +2641,23 @@
           <t>python</t>
         </is>
       </c>
-      <c r="E91" s="1" t="n">
+      <c r="E91" s="2" t="n">
         <v>45643.50651620371</v>
       </c>
       <c r="F91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>data[data["rating"] &gt; 8]</t>
+          <t>data[data["type"].isin(["TV", "Movie"])]</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Фильтрация по значению</t>
+          <t>Для получения строк датафрейма в ситуации, когда имеется список значений столбцов, можно воспользоваться следующей командой</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
@@ -2633,23 +2665,23 @@
           <t>python</t>
         </is>
       </c>
-      <c r="E92" s="1" t="n">
+      <c r="E92" s="2" t="n">
         <v>45643.50651620371</v>
       </c>
       <c r="F92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>data.sort_values("rating", ascending=False)</t>
+          <t>data[data["rating"] &gt; 8]</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Сортировка</t>
+          <t>Фильтрация по значению</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
@@ -2657,23 +2689,23 @@
           <t>python</t>
         </is>
       </c>
-      <c r="E93" s="1" t="n">
+      <c r="E93" s="2" t="n">
         <v>45643.50651620371</v>
       </c>
       <c r="F93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>data.groupby("type").count()</t>
+          <t>data.sort_values("rating", ascending=False)</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Функция df.groupby и подсчёт количества записей</t>
+          <t>Сортировка</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
@@ -2681,23 +2713,23 @@
           <t>python</t>
         </is>
       </c>
-      <c r="E94" s="1" t="n">
+      <c r="E94" s="2" t="n">
         <v>45643.50651620371</v>
       </c>
       <c r="F94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>data_modified.loc[["Haikyuu!! Second Season","Gintama"]]</t>
+          <t>data.groupby("type").count()</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Получение строк с нужными индексными значениями</t>
+          <t>Функция df.groupby и подсчёт количества записей</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -2705,23 +2737,23 @@
           <t>python</t>
         </is>
       </c>
-      <c r="E95" s="1" t="n">
+      <c r="E95" s="2" t="n">
         <v>45643.50651620371</v>
       </c>
       <c r="F95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>rating.merge(data, left_on=’data_id’, right_on=’data_id’, suffixes=(‘_left’, ‘_right’))</t>
+          <t>data_modified.loc[["Haikyuu!! Second Season","Gintama"]]</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Слияние датафреймов</t>
+          <t>Получение строк с нужными индексными значениями</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -2729,23 +2761,23 @@
           <t>python</t>
         </is>
       </c>
-      <c r="E96" s="1" t="n">
+      <c r="E96" s="2" t="n">
         <v>45643.50651620371</v>
       </c>
       <c r="F96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>data.info()</t>
+          <t>rating.merge(data, left_on=’data_id’, right_on=’data_id’, suffixes=(‘_left’, ‘_right’))</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Получение сведений о датафрейм</t>
+          <t>Слияние датафреймов</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -2753,23 +2785,23 @@
           <t>python</t>
         </is>
       </c>
-      <c r="E97" s="1" t="n">
+      <c r="E97" s="2" t="n">
         <v>45643.50651620371</v>
       </c>
       <c r="F97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>data.head()</t>
+          <t>data.info()</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Вывести первые пять строк датасета</t>
+          <t>Получение сведений о датафрейм</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
@@ -2777,23 +2809,23 @@
           <t>python</t>
         </is>
       </c>
-      <c r="E98" s="1" t="n">
+      <c r="E98" s="2" t="n">
         <v>45643.50651620371</v>
       </c>
       <c r="F98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>data.drop(["density","members"], axis="columns")</t>
+          <t>data.head()</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Удаление нескольких столбцов</t>
+          <t>Вывести первые пять строк датасета</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
@@ -2801,23 +2833,23 @@
           <t>python</t>
         </is>
       </c>
-      <c r="E99" s="1" t="n">
+      <c r="E99" s="2" t="n">
         <v>45643.50651620371</v>
       </c>
       <c r="F99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>data = data.rename(columns={"Country Code": "country_code"})</t>
+          <t>data.drop(["density","members"], axis="columns")</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Переименование столбца</t>
+          <t>Удаление нескольких столбцов</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -2825,23 +2857,23 @@
           <t>python</t>
         </is>
       </c>
-      <c r="E100" s="1" t="n">
+      <c r="E100" s="2" t="n">
         <v>45643.50651620371</v>
       </c>
       <c r="F100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>data.shape</t>
+          <t>data = data.rename(columns={"Country Code": "country_code"})</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Вывести количество строк и столбцов датасета</t>
+          <t>Переименование столбца</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
@@ -2849,23 +2881,23 @@
           <t>python</t>
         </is>
       </c>
-      <c r="E101" s="1" t="n">
+      <c r="E101" s="2" t="n">
         <v>45643.50651620371</v>
       </c>
       <c r="F101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>data.max()</t>
+          <t>data.shape</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>Получим максимальные значения в каждом столбце</t>
+          <t>Вывести количество строк и столбцов датасета</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -2873,23 +2905,23 @@
           <t>python</t>
         </is>
       </c>
-      <c r="E102" s="1" t="n">
+      <c r="E102" s="2" t="n">
         <v>45643.50651620371</v>
       </c>
       <c r="F102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>data_convert = data.astype("int16")</t>
+          <t>data.max()</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Изменение типа столбца</t>
+          <t>Получим максимальные значения в каждом столбце</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
@@ -2897,23 +2929,23 @@
           <t>python</t>
         </is>
       </c>
-      <c r="E103" s="1" t="n">
+      <c r="E103" s="2" t="n">
         <v>45643.50651620371</v>
       </c>
       <c r="F103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>df = pd.DataFrame(lst, columns=[c[0] for c in cur.description])</t>
+          <t>data_convert = data.astype("int16")</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>Создание датафрейма из базы данных</t>
+          <t>Изменение типа столбца</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -2921,23 +2953,23 @@
           <t>python</t>
         </is>
       </c>
-      <c r="E104" s="1" t="n">
+      <c r="E104" s="2" t="n">
         <v>45643.50651620371</v>
       </c>
       <c r="F104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>df = pd.read_excel('sotr.xlsx', index_col=0)</t>
+          <t>df = pd.DataFrame(lst, columns=[c[0] for c in cur.description])</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Загрузка данных из EXCEL файла</t>
+          <t>Создание датафрейма из базы данных</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -2945,23 +2977,23 @@
           <t>python</t>
         </is>
       </c>
-      <c r="E105" s="1" t="n">
+      <c r="E105" s="2" t="n">
         <v>45643.50651620371</v>
       </c>
       <c r="F105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>data = pd.read_csv("data.csv")</t>
+          <t>df = pd.read_excel('sotr.xlsx', index_col=0)</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>Загрузка CSV-данных в датафрейм</t>
+          <t>Загрузка данных из EXCEL файла</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -2969,73 +3001,73 @@
           <t>python</t>
         </is>
       </c>
-      <c r="E106" s="1" t="n">
+      <c r="E106" s="2" t="n">
         <v>45643.50651620371</v>
       </c>
       <c r="F106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
+        <v>111</v>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>data = pd.read_csv("data.csv")</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>Загрузка CSV-данных в датафрейм</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>python</t>
+        </is>
+      </c>
+      <c r="E107" s="2" t="n">
+        <v>45643.50651620371</v>
+      </c>
+      <c r="F107" t="inlineStr"/>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
         <v>118</v>
       </c>
-      <c r="B107" t="inlineStr">
+      <c r="B108" t="inlineStr">
         <is>
           <t>import datetime
 dt_now = datetime.datetime.now()
 print(dt_now)</t>
         </is>
       </c>
-      <c r="C107" t="inlineStr">
+      <c r="C108" t="inlineStr">
         <is>
           <t>Вывод текущей даты и времени.</t>
         </is>
       </c>
-      <c r="D107" t="inlineStr">
+      <c r="D108" t="inlineStr">
         <is>
           <t>python</t>
         </is>
       </c>
-      <c r="E107" s="1" t="n">
+      <c r="E108" s="2" t="n">
         <v>45643.50651620371</v>
-      </c>
-      <c r="F107" t="inlineStr"/>
-    </row>
-    <row r="108">
-      <c r="A108" t="n">
-        <v>119</v>
-      </c>
-      <c r="B108" t="inlineStr">
-        <is>
-          <t>INSERT INTO git_and_bash (command, name) VALUES ('test', 'test')</t>
-        </is>
-      </c>
-      <c r="C108" t="inlineStr">
-        <is>
-          <t>Добавление новой записи в таблицу</t>
-        </is>
-      </c>
-      <c r="D108" t="inlineStr">
-        <is>
-          <t>sql</t>
-        </is>
-      </c>
-      <c r="E108" s="1" t="n">
-        <v>45643.52030092593</v>
       </c>
       <c r="F108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>SELECT * FROM git_and_bash WHERE command LIKE '%ls%'</t>
+          <t>INSERT INTO git_and_bash (command, name) VALUES ('test', 'test')</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>Поиск в поле значений по части слова</t>
+          <t>Добавление новой записи в таблицу</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -3043,23 +3075,23 @@
           <t>sql</t>
         </is>
       </c>
-      <c r="E109" s="1" t="n">
+      <c r="E109" s="2" t="n">
         <v>45643.52030092593</v>
       </c>
       <c r="F109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>SELECT * FROM links ORDER BY id DESC</t>
+          <t>SELECT * FROM git_and_bash WHERE command LIKE '%ls%'</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>Сортировка всех записей по убыванию</t>
+          <t>Поиск в поле значений по части слова</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -3067,23 +3099,23 @@
           <t>sql</t>
         </is>
       </c>
-      <c r="E110" s="1" t="n">
+      <c r="E110" s="2" t="n">
         <v>45643.52030092593</v>
       </c>
       <c r="F110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>SELECT * FROM links ORDER BY id ASC</t>
+          <t>SELECT * FROM links ORDER BY id DESC</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>Сортировка по возрастанию</t>
+          <t>Сортировка всех записей по убыванию</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
@@ -3091,23 +3123,23 @@
           <t>sql</t>
         </is>
       </c>
-      <c r="E111" s="1" t="n">
+      <c r="E111" s="2" t="n">
         <v>45643.52030092593</v>
       </c>
       <c r="F111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>DELETE FROM git_and_bash WHERE id = 45</t>
+          <t>SELECT * FROM links ORDER BY id ASC</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>Удаление определенной записи</t>
+          <t>Сортировка по возрастанию</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
@@ -3115,23 +3147,23 @@
           <t>sql</t>
         </is>
       </c>
-      <c r="E112" s="1" t="n">
+      <c r="E112" s="2" t="n">
         <v>45643.52030092593</v>
       </c>
       <c r="F112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>DELETE FROM [train];</t>
+          <t>DELETE FROM git_and_bash WHERE id = 45</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>Очистка таблицы</t>
+          <t>Удаление определенной записи</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
@@ -3139,23 +3171,23 @@
           <t>sql</t>
         </is>
       </c>
-      <c r="E113" s="1" t="n">
+      <c r="E113" s="2" t="n">
         <v>45643.52030092593</v>
       </c>
       <c r="F113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>UPDATE [sql] SET [name]='Сортировка всех записей по убыванию' WHERE ([sql].[id] = 3);</t>
+          <t>DELETE FROM [train];</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>Изменение значения записи определенного поля</t>
+          <t>Очистка таблицы</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
@@ -3163,23 +3195,23 @@
           <t>sql</t>
         </is>
       </c>
-      <c r="E114" s="1" t="n">
+      <c r="E114" s="2" t="n">
         <v>45643.52030092593</v>
       </c>
       <c r="F114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>ALTER TABLE [train] ADD [imya] VARCHAR(250) NOT NULL;</t>
+          <t>UPDATE [sql] SET [name]='Сортировка всех записей по убыванию' WHERE ([sql].[id] = 3);</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>Добавление поля в таблицу</t>
+          <t>Изменение значения записи определенного поля</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
@@ -3187,23 +3219,23 @@
           <t>sql</t>
         </is>
       </c>
-      <c r="E115" s="1" t="n">
+      <c r="E115" s="2" t="n">
         <v>45643.52030092593</v>
       </c>
       <c r="F115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>ALTER TABLE [train] RENAME COLUMN [train_name] TO [familia];</t>
+          <t>ALTER TABLE [train] ADD [imya] VARCHAR(250) NOT NULL;</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>Переименование поля таблицы</t>
+          <t>Добавление поля в таблицу</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
@@ -3211,23 +3243,23 @@
           <t>sql</t>
         </is>
       </c>
-      <c r="E116" s="1" t="n">
+      <c r="E116" s="2" t="n">
         <v>45643.52030092593</v>
       </c>
       <c r="F116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>DROP TABLE [train];</t>
+          <t>ALTER TABLE [train] RENAME COLUMN [train_name] TO [familia];</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>Удаляет таблицу базы данных</t>
+          <t>Переименование поля таблицы</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
@@ -3235,23 +3267,23 @@
           <t>sql</t>
         </is>
       </c>
-      <c r="E117" s="1" t="n">
+      <c r="E117" s="2" t="n">
         <v>45643.52030092593</v>
       </c>
       <c r="F117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>SELECT DISTINCT field FROM table;</t>
+          <t>DROP TABLE [train];</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Поиск уникальных значений</t>
+          <t>Удаляет таблицу базы данных</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
@@ -3259,23 +3291,23 @@
           <t>sql</t>
         </is>
       </c>
-      <c r="E118" s="1" t="n">
+      <c r="E118" s="2" t="n">
         <v>45643.52030092593</v>
       </c>
       <c r="F118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>SELECT * FROM table;</t>
+          <t>SELECT DISTINCT field FROM table;</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>Вывод всех записей таблицы</t>
+          <t>Поиск уникальных значений</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
@@ -3283,16 +3315,40 @@
           <t>sql</t>
         </is>
       </c>
-      <c r="E119" s="1" t="n">
+      <c r="E119" s="2" t="n">
         <v>45643.52030092593</v>
       </c>
       <c r="F119" t="inlineStr"/>
     </row>
     <row r="120">
       <c r="A120" t="n">
+        <v>130</v>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>SELECT * FROM table;</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>Вывод всех записей таблицы</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>sql</t>
+        </is>
+      </c>
+      <c r="E120" s="2" t="n">
+        <v>45643.52030092593</v>
+      </c>
+      <c r="F120" t="inlineStr"/>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
         <v>131</v>
       </c>
-      <c r="B120" t="inlineStr">
+      <c r="B121" t="inlineStr">
         <is>
           <t>CREATE TABLE IF NOT EXISTS tasks (
   task_id INTEGER PRIMARY KEY AUTOINCREMENT,
@@ -3302,57 +3358,37 @@
 );</t>
         </is>
       </c>
-      <c r="C120" t="inlineStr">
-        <is>
-          <t>Создание таблицы в базе данных.</t>
-        </is>
-      </c>
-      <c r="D120" t="inlineStr">
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>Создание таблицы в базе данных</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
         <is>
           <t>sql</t>
         </is>
       </c>
-      <c r="E120" s="1" t="n">
+      <c r="E121" s="2" t="n">
         <v>45643.52030092593</v>
       </c>
-      <c r="F120" t="inlineStr"/>
-    </row>
-    <row r="121">
-      <c r="A121" t="n">
-        <v>132</v>
-      </c>
-      <c r="B121" t="inlineStr">
-        <is>
-          <t>dir jupyter-notebooks/</t>
-        </is>
-      </c>
-      <c r="C121" t="inlineStr">
-        <is>
-          <t>Выводит содержимое папки из текущей директории</t>
-        </is>
-      </c>
-      <c r="D121" t="inlineStr">
-        <is>
-          <t>cli</t>
-        </is>
-      </c>
-      <c r="E121" s="1" t="n">
-        <v>45644.68768518518</v>
-      </c>
-      <c r="F121" t="inlineStr"/>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>2025-01-21 15:11:03</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>git remote set-url origin git@github.com:savinsyu/flask-project-one-table-version.git  git add .  git commit -m "First commit"  git push -u origin main</t>
+          <t>dir jupyter-notebooks/</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>Команда для установки привязки к удаленному репозиторию.</t>
+          <t>Выводит содержимое папки из текущей директории</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
@@ -3360,23 +3396,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E122" s="1" t="n">
-        <v>45644.69016203703</v>
+      <c r="E122" s="2" t="n">
+        <v>45644.68768518518</v>
       </c>
       <c r="F122" t="inlineStr"/>
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>echo $RANDOM</t>
+          <t>git remote set-url origin git@github.com:savinsyu/flask-project-one-table-version.git  git add .  git commit -m "First commit"  git push -u origin main</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>Генерация случайных чисел с терминала</t>
+          <t>Команда для установки привязки к удаленному репозиторию.</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
@@ -3384,23 +3420,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E123" s="1" t="n">
-        <v>45649.41765046296</v>
+      <c r="E123" s="2" t="n">
+        <v>45644.69016203703</v>
       </c>
       <c r="F123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>sleep 1m</t>
+          <t>echo $RANDOM</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>Задержка в терминале, в данном случае на 1 минуту, s - секунды по умолчанию, m - минуты, h - час, d - день</t>
+          <t>Генерация случайных чисел с терминала</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
@@ -3408,23 +3444,23 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E124" s="1" t="n">
+      <c r="E124" s="2" t="n">
         <v>45649.41765046296</v>
       </c>
       <c r="F124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>echo "Hello world!" &gt;&gt; hello_world.txt</t>
+          <t>sleep 1m</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>Создается текстовый файл с текстом Hello World</t>
+          <t>Задержка в терминале, в данном случае на 1 минуту, s - секунды по умолчанию, m - минуты, h - час, d - день</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
@@ -3432,34 +3468,58 @@
           <t>cli</t>
         </is>
       </c>
-      <c r="E125" s="1" t="n">
-        <v>45650.61358796297</v>
+      <c r="E125" s="2" t="n">
+        <v>45649.41765046296</v>
       </c>
       <c r="F125" t="inlineStr"/>
     </row>
     <row r="126">
       <c r="A126" t="n">
+        <v>136</v>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>echo "Hello world!" &gt;&gt; hello_world.txt</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>Создается текстовый файл с текстом Hello World</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>cli</t>
+        </is>
+      </c>
+      <c r="E126" s="2" t="n">
+        <v>45650.61358796297</v>
+      </c>
+      <c r="F126" t="inlineStr"/>
+    </row>
+    <row r="127">
+      <c r="A127" t="n">
         <v>146</v>
       </c>
-      <c r="B126" t="inlineStr">
+      <c r="B127" t="inlineStr">
         <is>
           <t>cd /g</t>
         </is>
       </c>
-      <c r="C126" t="inlineStr">
+      <c r="C127" t="inlineStr">
         <is>
           <t>Переход на другой диск, в данном случае диск g:</t>
         </is>
       </c>
-      <c r="D126" t="inlineStr">
-        <is>
-          <t>cli</t>
-        </is>
-      </c>
-      <c r="E126" s="1" t="n">
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>cli</t>
+        </is>
+      </c>
+      <c r="E127" s="2" t="n">
         <v>45677.64894675926</v>
       </c>
-      <c r="F126" t="inlineStr"/>
+      <c r="F127" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>